<commit_message>
Aggiunte nuove analisi e lo script per calcolare la correlazione
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeT5_225.xlsx
+++ b/HE/W_in_progress/AnalisiCodeT5_225.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61396E96-43D8-4C9B-A42C-23F97754E3A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF05D8D1-F7D2-4121-ACC9-8195EFE3574B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="834">
   <si>
     <t>IN</t>
   </si>
@@ -1116,6 +1116,9 @@
     <t>debouncer_display_btn: button_debouncer port map(clk_period =&gt; 10, btn_noise_time =&gt; 10000000);</t>
   </si>
   <si>
+    <t>Manca gli altri parametri</t>
+  </si>
+  <si>
     <t>debouncer_plaintext_btn is an instance of button_debouncer with parameters clk_period set to 10, btn_noise_time set to 10000000 and signals rst, clock, btn_plainText_in, t_btn_plaintext are connected</t>
   </si>
   <si>
@@ -1242,6 +1245,9 @@
     <t>constant LATCH_CNT : boolean := false; if clatch = 0 then LATCH_CNT &lt;= true; else LATCH_CNT &lt;= false; end if;</t>
   </si>
   <si>
+    <t>Equivalente</t>
+  </si>
+  <si>
     <t>n is a constant of type integer initialized to 1000</t>
   </si>
   <si>
@@ -1278,6 +1284,9 @@
     <t>gen_rx_ddr_lvds : for i in 0 to 4 generate inst_IDDR : IDDR generic map (DR_CLK_EDGE =&gt; "SAME_EDGE_PIPELINED", SRTYPE =&gt; "ASYNC") port map (Q1 =&gt; rx_data_3x_i(i), Q2 =&gt; rx_data_3x_q(i), C =&gt; clk_rx_3x, CE =&gt; '1', D =&gt; rx_data_3x_ddr(i), R =&gt; rx_reset, S =&gt; '0'); inst_IBUFDS : IBUFDS generic map (DIFF_TERM =&gt; TRUE, IOSTANDARD =&gt; "DEFAULT") port map (I =&gt; RX_DATA_P(i), IB =&gt; RX_DATA_N(i), O =&gt; rx_data_3x_ddr(i)); end generate;</t>
   </si>
   <si>
+    <t>Quasi identici</t>
+  </si>
+  <si>
     <t>gen_num is a for generate statement on variable N over LOOP_COUNT range that generates component rd_gen_inst2 that is an instance of fifo_rng with generic signals WIDTH initialized to 8, SEED initialized to TB_SEED+N and port signals CLK initialized to RD_CLK, RESET initialized to RESET, RANDOM_NUM initialized to elements of rand_num with indices from 8*(N+1)-1 down to 8*N, ENABLE initialized to pr_r_en</t>
   </si>
   <si>
@@ -1285,6 +1294,9 @@
   </si>
   <si>
     <t>gen_num: for N in 0 to LOOP_COUNT range generate rd_gen_inst2: rd_gen_generic port map (WIDTH =&gt; 8, SEED =&gt; TB_SEED+N, CLK =&gt; RD_CLK, RESET =&gt; RESET, RANDOM_NUM =&gt; rand_num(8*(N+1)-1 downto 8*N), ENABLE =&gt; pr_r_en); end generate;</t>
+  </si>
+  <si>
+    <t>Piccoli errori sulla sintassi, però più o meno fa quello che è stato chiesto</t>
   </si>
   <si>
     <t>define a signal round_keys as an array of dataArrayType</t>
@@ -2885,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
-      <selection activeCell="C327" sqref="C327"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="G177" sqref="G177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6258,7 +6270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>342</v>
       </c>
@@ -6281,7 +6293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>345</v>
       </c>
@@ -6304,7 +6316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>347</v>
       </c>
@@ -6327,7 +6339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>350</v>
       </c>
@@ -6350,7 +6362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>352</v>
       </c>
@@ -6373,7 +6385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>355</v>
       </c>
@@ -6396,7 +6408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>358</v>
       </c>
@@ -6418,16 +6430,19 @@
       <c r="G151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:7">
+      <c r="H151" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B152" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C152" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -6439,18 +6454,18 @@
         <v>0.99997722303206993</v>
       </c>
       <c r="G152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B153" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C153" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D153">
         <v>1</v>
@@ -6465,15 +6480,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B154" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C154" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D154">
         <v>1</v>
@@ -6488,15 +6503,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B155" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C155" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D155">
         <v>1</v>
@@ -6511,15 +6526,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:8">
       <c r="A156" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B156" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C156" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D156">
         <v>1</v>
@@ -6534,15 +6549,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:8">
       <c r="A157" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B157" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C157" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D157">
         <v>1</v>
@@ -6557,15 +6572,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:8">
       <c r="A158" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B158" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C158" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -6577,18 +6592,18 @@
         <v>0.9999941303531179</v>
       </c>
       <c r="G158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
       <c r="A159" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B159" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C159" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -6600,18 +6615,18 @@
         <v>0.99999218749999996</v>
       </c>
       <c r="G159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
       <c r="A160" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B160" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C160" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -6623,18 +6638,18 @@
         <v>0.99997155211652256</v>
       </c>
       <c r="G160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
       <c r="A161" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B161" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C161" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D161">
         <v>1</v>
@@ -6649,15 +6664,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B162" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C162" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -6672,15 +6687,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B163" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C163" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D163">
         <v>1</v>
@@ -6695,15 +6710,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B164" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C164" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D164">
         <v>1</v>
@@ -6718,15 +6733,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B165" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C165" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D165">
         <v>1</v>
@@ -6741,15 +6756,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B166" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C166" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D166">
         <v>1</v>
@@ -6764,15 +6779,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B167" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C167" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -6784,18 +6799,18 @@
         <v>0.88194444444444442</v>
       </c>
       <c r="G167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B168" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C168" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -6810,15 +6825,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B169" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C169" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -6830,18 +6845,21 @@
         <v>0.58826632900706977</v>
       </c>
       <c r="G169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H169" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B170" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C170" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D170">
         <v>1</v>
@@ -6856,15 +6874,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B171" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C171" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D171">
         <v>1</v>
@@ -6879,15 +6897,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B172" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C172" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -6899,18 +6917,18 @@
         <v>0.88194444444444442</v>
       </c>
       <c r="G172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B173" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C173" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -6925,15 +6943,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B174" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C174" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D174">
         <v>1</v>
@@ -6948,15 +6966,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B175" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C175" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -6968,18 +6986,21 @@
         <v>0.99230584330638416</v>
       </c>
       <c r="G175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H175" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="B176" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C176" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -6991,12 +7012,15 @@
         <v>0.89218192045587219</v>
       </c>
       <c r="G176">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H176" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="177" spans="1:7">
       <c r="A177" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B177" t="s">
         <v>109</v>
@@ -7019,13 +7043,13 @@
     </row>
     <row r="178" spans="1:7">
       <c r="A178" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="B178" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C178" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -7042,13 +7066,13 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B179" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C179" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -7065,13 +7089,13 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180" t="s">
+        <v>429</v>
+      </c>
+      <c r="B180" t="s">
+        <v>424</v>
+      </c>
+      <c r="C180" t="s">
         <v>425</v>
-      </c>
-      <c r="B180" t="s">
-        <v>420</v>
-      </c>
-      <c r="C180" t="s">
-        <v>421</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -7088,13 +7112,13 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B181" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C181" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="D181">
         <v>1</v>
@@ -7111,13 +7135,13 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B182" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C182" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -7134,13 +7158,13 @@
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="B183" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="C183" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -7157,13 +7181,13 @@
     </row>
     <row r="184" spans="1:7">
       <c r="A184" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="B184" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="C184" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D184">
         <v>1</v>
@@ -7180,13 +7204,13 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B185" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C185" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D185">
         <v>1</v>
@@ -7203,13 +7227,13 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="B186" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C186" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -7226,13 +7250,13 @@
     </row>
     <row r="187" spans="1:7">
       <c r="A187" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B187" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C187" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -7249,13 +7273,13 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B188" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="C188" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -7272,13 +7296,13 @@
     </row>
     <row r="189" spans="1:7">
       <c r="A189" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B189" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C189" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -7295,13 +7319,13 @@
     </row>
     <row r="190" spans="1:7">
       <c r="A190" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B190" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C190" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="D190">
         <v>1</v>
@@ -7318,13 +7342,13 @@
     </row>
     <row r="191" spans="1:7">
       <c r="A191" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B191" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C191" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -7341,13 +7365,13 @@
     </row>
     <row r="192" spans="1:7">
       <c r="A192" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B192" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C192" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D192">
         <v>1</v>
@@ -7364,13 +7388,13 @@
     </row>
     <row r="193" spans="1:7">
       <c r="A193" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B193" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C193" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="D193">
         <v>0</v>
@@ -7387,13 +7411,13 @@
     </row>
     <row r="194" spans="1:7">
       <c r="A194" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B194" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C194" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="D194">
         <v>1</v>
@@ -7410,13 +7434,13 @@
     </row>
     <row r="195" spans="1:7">
       <c r="A195" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B195" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C195" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -7433,13 +7457,13 @@
     </row>
     <row r="196" spans="1:7">
       <c r="A196" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B196" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="C196" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D196">
         <v>1</v>
@@ -7456,13 +7480,13 @@
     </row>
     <row r="197" spans="1:7">
       <c r="A197" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B197" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="C197" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -7479,13 +7503,13 @@
     </row>
     <row r="198" spans="1:7">
       <c r="A198" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B198" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C198" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="D198">
         <v>1</v>
@@ -7502,13 +7526,13 @@
     </row>
     <row r="199" spans="1:7">
       <c r="A199" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B199" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C199" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -7525,13 +7549,13 @@
     </row>
     <row r="200" spans="1:7">
       <c r="A200" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B200" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C200" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -7548,13 +7572,13 @@
     </row>
     <row r="201" spans="1:7">
       <c r="A201" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B201" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C201" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -7571,13 +7595,13 @@
     </row>
     <row r="202" spans="1:7">
       <c r="A202" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B202" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C202" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -7594,13 +7618,13 @@
     </row>
     <row r="203" spans="1:7">
       <c r="A203" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B203" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C203" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -7617,13 +7641,13 @@
     </row>
     <row r="204" spans="1:7">
       <c r="A204" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="B204" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C204" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -7640,13 +7664,13 @@
     </row>
     <row r="205" spans="1:7">
       <c r="A205" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B205" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C205" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -7663,13 +7687,13 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="B206" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C206" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -7686,13 +7710,13 @@
     </row>
     <row r="207" spans="1:7">
       <c r="A207" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B207" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C207" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -7709,13 +7733,13 @@
     </row>
     <row r="208" spans="1:7">
       <c r="A208" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="B208" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C208" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D208">
         <v>1</v>
@@ -7732,13 +7756,13 @@
     </row>
     <row r="209" spans="1:7">
       <c r="A209" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="B209" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C209" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -7755,13 +7779,13 @@
     </row>
     <row r="210" spans="1:7">
       <c r="A210" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B210" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="C210" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="D210">
         <v>0</v>
@@ -7778,13 +7802,13 @@
     </row>
     <row r="211" spans="1:7">
       <c r="A211" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B211" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="C211" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -7801,13 +7825,13 @@
     </row>
     <row r="212" spans="1:7">
       <c r="A212" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="B212" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="C212" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="D212">
         <v>1</v>
@@ -7824,13 +7848,13 @@
     </row>
     <row r="213" spans="1:7">
       <c r="A213" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="B213" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="C213" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -7847,13 +7871,13 @@
     </row>
     <row r="214" spans="1:7">
       <c r="A214" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="B214" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="C214" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="D214">
         <v>1</v>
@@ -7870,13 +7894,13 @@
     </row>
     <row r="215" spans="1:7">
       <c r="A215" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="B215" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="C215" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D215">
         <v>1</v>
@@ -7893,13 +7917,13 @@
     </row>
     <row r="216" spans="1:7">
       <c r="A216" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="B216" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="C216" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -7916,13 +7940,13 @@
     </row>
     <row r="217" spans="1:7">
       <c r="A217" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="B217" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="C217" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="D217">
         <v>1</v>
@@ -7939,13 +7963,13 @@
     </row>
     <row r="218" spans="1:7">
       <c r="A218" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="B218" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="C218" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -7962,13 +7986,13 @@
     </row>
     <row r="219" spans="1:7">
       <c r="A219" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B219" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="C219" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -7985,13 +8009,13 @@
     </row>
     <row r="220" spans="1:7">
       <c r="A220" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="B220" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="C220" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -8008,13 +8032,13 @@
     </row>
     <row r="221" spans="1:7">
       <c r="A221" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B221" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="C221" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="D221">
         <v>1</v>
@@ -8031,13 +8055,13 @@
     </row>
     <row r="222" spans="1:7">
       <c r="A222" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="B222" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="C222" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="D222">
         <v>1</v>
@@ -8054,13 +8078,13 @@
     </row>
     <row r="223" spans="1:7">
       <c r="A223" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="B223" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="C223" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="D223">
         <v>1</v>
@@ -8077,13 +8101,13 @@
     </row>
     <row r="224" spans="1:7">
       <c r="A224" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="B224" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="C224" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D224">
         <v>0</v>
@@ -8100,13 +8124,13 @@
     </row>
     <row r="225" spans="1:7">
       <c r="A225" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="B225" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="C225" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="D225">
         <v>0</v>
@@ -8123,13 +8147,13 @@
     </row>
     <row r="226" spans="1:7">
       <c r="A226" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B226" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="C226" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="D226">
         <v>0</v>
@@ -8146,13 +8170,13 @@
     </row>
     <row r="227" spans="1:7">
       <c r="A227" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B227" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C227" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="D227">
         <v>0</v>
@@ -8169,13 +8193,13 @@
     </row>
     <row r="228" spans="1:7">
       <c r="A228" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="B228" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="C228" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="D228">
         <v>0</v>
@@ -8192,13 +8216,13 @@
     </row>
     <row r="229" spans="1:7">
       <c r="A229" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B229" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="C229" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="D229">
         <v>0</v>
@@ -8215,13 +8239,13 @@
     </row>
     <row r="230" spans="1:7">
       <c r="A230" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="B230" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="C230" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="D230">
         <v>0</v>
@@ -8238,13 +8262,13 @@
     </row>
     <row r="231" spans="1:7">
       <c r="A231" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B231" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="C231" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="D231">
         <v>0</v>
@@ -8261,13 +8285,13 @@
     </row>
     <row r="232" spans="1:7">
       <c r="A232" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="B232" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="C232" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="D232">
         <v>0</v>
@@ -8284,13 +8308,13 @@
     </row>
     <row r="233" spans="1:7">
       <c r="A233" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B233" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="C233" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="D233">
         <v>0</v>
@@ -8307,13 +8331,13 @@
     </row>
     <row r="234" spans="1:7">
       <c r="A234" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="B234" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="C234" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="D234">
         <v>0</v>
@@ -8330,13 +8354,13 @@
     </row>
     <row r="235" spans="1:7">
       <c r="A235" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="B235" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="C235" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="D235">
         <v>0</v>
@@ -8353,13 +8377,13 @@
     </row>
     <row r="236" spans="1:7">
       <c r="A236" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="B236" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="C236" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -8376,13 +8400,13 @@
     </row>
     <row r="237" spans="1:7">
       <c r="A237" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="B237" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="C237" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -8399,13 +8423,13 @@
     </row>
     <row r="238" spans="1:7">
       <c r="A238" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="B238" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="C238" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -8422,13 +8446,13 @@
     </row>
     <row r="239" spans="1:7">
       <c r="A239" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="B239" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="C239" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -8445,13 +8469,13 @@
     </row>
     <row r="240" spans="1:7">
       <c r="A240" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="B240" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="C240" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -8468,13 +8492,13 @@
     </row>
     <row r="241" spans="1:7">
       <c r="A241" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="B241" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="C241" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -8491,13 +8515,13 @@
     </row>
     <row r="242" spans="1:7">
       <c r="A242" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="B242" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="C242" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -8514,13 +8538,13 @@
     </row>
     <row r="243" spans="1:7">
       <c r="A243" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="B243" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="C243" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -8537,13 +8561,13 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="B244" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="C244" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -8560,13 +8584,13 @@
     </row>
     <row r="245" spans="1:7">
       <c r="A245" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B245" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="C245" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -8583,13 +8607,13 @@
     </row>
     <row r="246" spans="1:7">
       <c r="A246" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="B246" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="C246" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -8606,13 +8630,13 @@
     </row>
     <row r="247" spans="1:7">
       <c r="A247" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="B247" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="C247" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -8629,13 +8653,13 @@
     </row>
     <row r="248" spans="1:7">
       <c r="A248" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="B248" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="C248" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -8652,13 +8676,13 @@
     </row>
     <row r="249" spans="1:7">
       <c r="A249" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="B249" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="C249" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -8675,13 +8699,13 @@
     </row>
     <row r="250" spans="1:7">
       <c r="A250" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="B250" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="C250" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -8698,13 +8722,13 @@
     </row>
     <row r="251" spans="1:7">
       <c r="A251" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="B251" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="C251" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -8721,13 +8745,13 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B252" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="C252" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -8744,13 +8768,13 @@
     </row>
     <row r="253" spans="1:7">
       <c r="A253" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="B253" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="C253" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -8767,13 +8791,13 @@
     </row>
     <row r="254" spans="1:7">
       <c r="A254" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="B254" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="C254" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -8790,13 +8814,13 @@
     </row>
     <row r="255" spans="1:7">
       <c r="A255" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="B255" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="C255" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -8813,13 +8837,13 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="B256" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="C256" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -8836,13 +8860,13 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="B257" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="C257" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -8859,13 +8883,13 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="B258" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="C258" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -8882,13 +8906,13 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="B259" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="C259" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -8905,13 +8929,13 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="B260" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="C260" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -8928,13 +8952,13 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="B261" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="C261" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -8951,13 +8975,13 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="B262" t="s">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="C262" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -8974,13 +8998,13 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="B263" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="C263" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -8997,13 +9021,13 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="B264" t="s">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C264" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9020,13 +9044,13 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" t="s">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="B265" t="s">
-        <v>654</v>
+        <v>658</v>
       </c>
       <c r="C265" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9043,13 +9067,13 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="B266" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="C266" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9066,13 +9090,13 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="B267" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="C267" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9089,13 +9113,13 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="B268" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
       <c r="C268" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9112,13 +9136,13 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="B269" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="C269" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9135,13 +9159,13 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="B270" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="C270" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -9158,13 +9182,13 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="B271" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c r="C271" t="s">
-        <v>673</v>
+        <v>677</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9181,13 +9205,13 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="B272" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="C272" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -9204,13 +9228,13 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="B273" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="C273" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -9227,13 +9251,13 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="B274" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="C274" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -9250,13 +9274,13 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="B275" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="C275" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -9273,13 +9297,13 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="B276" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="C276" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9296,13 +9320,13 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="B277" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="C277" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -9319,13 +9343,13 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="B278" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="C278" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -9342,13 +9366,13 @@
     </row>
     <row r="279" spans="1:7">
       <c r="A279" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="B279" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="C279" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -9365,13 +9389,13 @@
     </row>
     <row r="280" spans="1:7">
       <c r="A280" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="B280" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="C280" t="s">
-        <v>699</v>
+        <v>703</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -9388,13 +9412,13 @@
     </row>
     <row r="281" spans="1:7">
       <c r="A281" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="B281" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="C281" t="s">
-        <v>701</v>
+        <v>705</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -9411,13 +9435,13 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="B282" t="s">
-        <v>703</v>
+        <v>707</v>
       </c>
       <c r="C282" t="s">
-        <v>704</v>
+        <v>708</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -9434,13 +9458,13 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283" t="s">
-        <v>705</v>
+        <v>709</v>
       </c>
       <c r="B283" t="s">
-        <v>706</v>
+        <v>710</v>
       </c>
       <c r="C283" t="s">
-        <v>707</v>
+        <v>711</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -9457,13 +9481,13 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" t="s">
-        <v>708</v>
+        <v>712</v>
       </c>
       <c r="B284" t="s">
-        <v>709</v>
+        <v>713</v>
       </c>
       <c r="C284" t="s">
-        <v>710</v>
+        <v>714</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -9480,13 +9504,13 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="B285" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="C285" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -9503,13 +9527,13 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="B286" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="C286" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -9526,13 +9550,13 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="B287" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="C287" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -9549,13 +9573,13 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="B288" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="C288" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -9572,13 +9596,13 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="B289" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="C289" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -9595,13 +9619,13 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c r="B290" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c r="C290" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -9618,13 +9642,13 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" t="s">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="B291" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="C291" t="s">
-        <v>729</v>
+        <v>733</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -9641,13 +9665,13 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="B292" t="s">
-        <v>731</v>
+        <v>735</v>
       </c>
       <c r="C292" t="s">
-        <v>732</v>
+        <v>736</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -9664,13 +9688,13 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" t="s">
-        <v>733</v>
+        <v>737</v>
       </c>
       <c r="B293" t="s">
-        <v>734</v>
+        <v>738</v>
       </c>
       <c r="C293" t="s">
-        <v>735</v>
+        <v>739</v>
       </c>
       <c r="D293">
         <v>0</v>
@@ -9687,13 +9711,13 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B294" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="C294" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -9710,13 +9734,13 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="B295" t="s">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="C295" t="s">
-        <v>741</v>
+        <v>745</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -9733,13 +9757,13 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="B296" t="s">
-        <v>743</v>
+        <v>747</v>
       </c>
       <c r="C296" t="s">
-        <v>744</v>
+        <v>748</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -9756,13 +9780,13 @@
     </row>
     <row r="297" spans="1:7">
       <c r="A297" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="B297" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="C297" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -9779,13 +9803,13 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" t="s">
-        <v>747</v>
+        <v>751</v>
       </c>
       <c r="B298" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="C298" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -9802,13 +9826,13 @@
     </row>
     <row r="299" spans="1:7">
       <c r="A299" t="s">
-        <v>750</v>
+        <v>754</v>
       </c>
       <c r="B299" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="C299" t="s">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -9825,13 +9849,13 @@
     </row>
     <row r="300" spans="1:7">
       <c r="A300" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="B300" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="C300" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -9848,13 +9872,13 @@
     </row>
     <row r="301" spans="1:7">
       <c r="A301" t="s">
-        <v>755</v>
+        <v>759</v>
       </c>
       <c r="B301" t="s">
-        <v>756</v>
+        <v>760</v>
       </c>
       <c r="C301" t="s">
-        <v>757</v>
+        <v>761</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -9871,13 +9895,13 @@
     </row>
     <row r="302" spans="1:7">
       <c r="A302" t="s">
-        <v>758</v>
+        <v>762</v>
       </c>
       <c r="B302" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
       <c r="C302" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -9894,13 +9918,13 @@
     </row>
     <row r="303" spans="1:7">
       <c r="A303" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="B303" t="s">
-        <v>762</v>
+        <v>766</v>
       </c>
       <c r="C303" t="s">
-        <v>763</v>
+        <v>767</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -9917,13 +9941,13 @@
     </row>
     <row r="304" spans="1:7">
       <c r="A304" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="B304" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="C304" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -9940,13 +9964,13 @@
     </row>
     <row r="305" spans="1:7">
       <c r="A305" t="s">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="B305" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="C305" t="s">
-        <v>768</v>
+        <v>772</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -9963,13 +9987,13 @@
     </row>
     <row r="306" spans="1:7">
       <c r="A306" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="B306" t="s">
-        <v>770</v>
+        <v>774</v>
       </c>
       <c r="C306" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -9986,13 +10010,13 @@
     </row>
     <row r="307" spans="1:7">
       <c r="A307" t="s">
-        <v>772</v>
+        <v>776</v>
       </c>
       <c r="B307" t="s">
-        <v>773</v>
+        <v>777</v>
       </c>
       <c r="C307" t="s">
-        <v>774</v>
+        <v>778</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10009,13 +10033,13 @@
     </row>
     <row r="308" spans="1:7">
       <c r="A308" t="s">
-        <v>775</v>
+        <v>779</v>
       </c>
       <c r="B308" t="s">
-        <v>776</v>
+        <v>780</v>
       </c>
       <c r="C308" t="s">
-        <v>777</v>
+        <v>781</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10032,13 +10056,13 @@
     </row>
     <row r="309" spans="1:7">
       <c r="A309" t="s">
-        <v>778</v>
+        <v>782</v>
       </c>
       <c r="B309" t="s">
-        <v>779</v>
+        <v>783</v>
       </c>
       <c r="C309" t="s">
-        <v>780</v>
+        <v>784</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10055,13 +10079,13 @@
     </row>
     <row r="310" spans="1:7">
       <c r="A310" t="s">
-        <v>781</v>
+        <v>785</v>
       </c>
       <c r="B310" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="C310" t="s">
-        <v>782</v>
+        <v>786</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -10078,13 +10102,13 @@
     </row>
     <row r="311" spans="1:7">
       <c r="A311" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="B311" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
       <c r="C311" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -10101,13 +10125,13 @@
     </row>
     <row r="312" spans="1:7">
       <c r="A312" t="s">
-        <v>786</v>
+        <v>790</v>
       </c>
       <c r="B312" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="C312" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="D312">
         <v>1</v>
@@ -10124,13 +10148,13 @@
     </row>
     <row r="313" spans="1:7">
       <c r="A313" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="B313" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="C313" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10147,13 +10171,13 @@
     </row>
     <row r="314" spans="1:7">
       <c r="A314" t="s">
-        <v>791</v>
+        <v>795</v>
       </c>
       <c r="B314" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="C314" t="s">
-        <v>793</v>
+        <v>797</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10170,13 +10194,13 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" t="s">
-        <v>794</v>
+        <v>798</v>
       </c>
       <c r="B315" t="s">
-        <v>795</v>
+        <v>799</v>
       </c>
       <c r="C315" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10193,13 +10217,13 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" t="s">
-        <v>797</v>
+        <v>801</v>
       </c>
       <c r="B316" t="s">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="C316" t="s">
-        <v>799</v>
+        <v>803</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10216,13 +10240,13 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" t="s">
-        <v>800</v>
+        <v>804</v>
       </c>
       <c r="B317" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="C317" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -10239,13 +10263,13 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="B318" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="C318" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10262,13 +10286,13 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="B319" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="C319" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10285,13 +10309,13 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="B320" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="C320" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -10308,13 +10332,13 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="B321" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="C321" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -10331,13 +10355,13 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="B322" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
       <c r="C322" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -10354,13 +10378,13 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="B323" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c r="C323" t="s">
-        <v>818</v>
+        <v>822</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -10377,13 +10401,13 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>819</v>
+        <v>823</v>
       </c>
       <c r="B324" t="s">
-        <v>820</v>
+        <v>824</v>
       </c>
       <c r="C324" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10400,13 +10424,13 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>822</v>
+        <v>826</v>
       </c>
       <c r="B325" t="s">
-        <v>823</v>
+        <v>827</v>
       </c>
       <c r="C325" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10423,13 +10447,13 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
       <c r="B326" t="s">
-        <v>826</v>
+        <v>830</v>
       </c>
       <c r="C326" t="s">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -10446,13 +10470,13 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>828</v>
+        <v>832</v>
       </c>
       <c r="B327" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="C327" t="s">
-        <v>829</v>
+        <v>833</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Aggiunte nuove analisi e aggiustato il framework
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeT5_225.xlsx
+++ b/HE/W_in_progress/AnalisiCodeT5_225.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B920AD3-94FC-4B26-A9DC-90D8B00BED6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC08C1E3-0180-4D84-8D6F-C07D29457173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="871">
   <si>
     <t>IN</t>
   </si>
@@ -1476,6 +1476,9 @@
     <t>assert clock_enable = '0' report "Clock enable not enabled" severity error when clock_enable = '1';</t>
   </si>
   <si>
+    <t>Sintatticamente non corretta</t>
+  </si>
+  <si>
     <t>Verify that 'output' is updated on the falling edge of 'clk' when 'enable' is high</t>
   </si>
   <si>
@@ -1485,6 +1488,9 @@
     <t>assert enable = '1' report "Output not updated on falling edge" severity error when clk_event = '1' and clk_event_type = '1' and enable = '1';</t>
   </si>
   <si>
+    <t>Non prevede l'evento</t>
+  </si>
+  <si>
     <t>Ensure 'reset' pulse width is at least 10 ns</t>
   </si>
   <si>
@@ -1494,6 +1500,9 @@
     <t>assert reset_pulse_width = 10 ns report "Reset pulse width too short" severity error;</t>
   </si>
   <si>
+    <t>Completamente sbagliata</t>
+  </si>
+  <si>
     <t>Check if 'data_out' matches expected pattern</t>
   </si>
   <si>
@@ -1503,6 +1512,9 @@
     <t>assert data_out matches expected_pattern report "Data out matches expected pattern" severity error;</t>
   </si>
   <si>
+    <t>Ha traslitterato</t>
+  </si>
+  <si>
     <t>Check if 'output' toggles every clock cycle when 'toggle_mode' is active</t>
   </si>
   <si>
@@ -1512,6 +1524,9 @@
     <t>assert output = '1' report "Output not toggled after toggle_mode" severity error;</t>
   </si>
   <si>
+    <t>Completamente sballato</t>
+  </si>
+  <si>
     <t>Report an error message with failure severity if the output signal does not equal '0'</t>
   </si>
   <si>
@@ -1530,6 +1545,9 @@
     <t>architecture archi of shift_register is begin process (clk) begin if rising_edge(clk) then shift_reg &lt;= shift_reg(3 downto 0) &amp; input; end if; end process;</t>
   </si>
   <si>
+    <t>Concatenazione non equivalente</t>
+  </si>
+  <si>
     <t>half_adder is the entity for the half adder</t>
   </si>
   <si>
@@ -1557,6 +1575,9 @@
     <t>entity decoder_2_4 is port(a0 : in STD_LOGIC; a1 : in STD_LOGIC; s : in STD_LOGIC; y : out STD_LOGIC); end decoder_2_4;</t>
   </si>
   <si>
+    <t>Non ha 4 uscite</t>
+  </si>
+  <si>
     <t>define the entity for a multiplier 8 bit</t>
   </si>
   <si>
@@ -1566,6 +1587,9 @@
     <t>entity multiplier_8 is port(clk, rst, si : in std_logic; so : out std_logic); end multiplier_8;</t>
   </si>
   <si>
+    <t>Non è un moltiplicatore</t>
+  </si>
+  <si>
     <t>define the variable size of type integer with values from 10 to 10000 and initialize it to 1000</t>
   </si>
   <si>
@@ -1656,6 +1680,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity glitch_filter is Port ( Noisy_In : in STD_LOGIC; Filtered_Out : out STD_LOGIC); end glitch_filter; architecture Behavioral of glitch_filter is begin process (Noisy_In) variable filtered_out : std_logic := '0'; begin filtered_out := Noisy_In; for i in 0 to 15 loop filtered_out := filtered_out(i) xor '1'; end loop ; Filtered_Out &lt;= filtered_out; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non fa il filtraggio dei glitch</t>
+  </si>
+  <si>
     <t>Implement a basic moving average filter with circular buffer</t>
   </si>
   <si>
@@ -1665,6 +1692,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then sum &lt;= (others =&gt; '0'); elsif sum = '0' then sum &lt;= '1'; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non implementa ciò che ho richeisto</t>
+  </si>
+  <si>
     <t>Implement a Manchester decoder using a process.</t>
   </si>
   <si>
@@ -1674,6 +1704,9 @@
     <t>process(clk,rst)begin if rst='1'then manchester_out&lt;='0';elsif rising_edge(clk)then manchester_out&lt;=not manchester_out;end if;end process;</t>
   </si>
   <si>
+    <t>E' un toggle</t>
+  </si>
+  <si>
     <t>Define a register of N-bit with the signals clock, reset, enable, and D (N-bit) as input and the signal Q (N-bit) as output.</t>
   </si>
   <si>
@@ -1683,6 +1716,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity Register is Generic(N : natural := 8); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Enable : in STD_LOGIC; D : in STD_LOGIC_VECTOR (N-1 downto 0); Q : out STD_LOGIC_VECTOR (N-1 downto 0)); end Register; architecture Behavioral of Register is begin process (Clock, Reset) variable reg : unsigned(N-1 downto 0); begin if (Reset = '1') then reg := (others =&gt; '0'); elsif (rising_edge(Clock)) then if (Enable = '1') then reg := reg(N-2 downto 0) &amp; D; end if ; end if ; Q &lt;= reg; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Fa un registro</t>
+  </si>
+  <si>
     <t>Create a simple 4-bit comparator</t>
   </si>
   <si>
@@ -1692,6 +1728,9 @@
     <t>process(a, b) begin if a = b then case state is when IDLE =&gt; if a = '1' and b = '0' then state &lt;= COMPARATOR; else state &lt;= COMPARATOR_IN; end if; when COMPARATOR_IN =&gt; if a = '1' and b = '0' then state &lt;= IDLE; else state &lt;= IDLE; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '0' then state &lt;= IDLE; else state &lt;= IDLE; end if; when IDLE =&gt; if a = '1' and b = '0' then state &lt;= COMPARATOR; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '0' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '1' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '0' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '1' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '0' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '1' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if a = '1' and b = '0' then state &lt;= IDLE; else state &lt;= COMPARATOR_OUT; end if; when COMPARATOR_OUT =&gt; if</t>
   </si>
   <si>
+    <t>Fa proprio un altra cosa</t>
+  </si>
+  <si>
     <t>Implement an SPI slave using a process.</t>
   </si>
   <si>
@@ -1701,6 +1740,9 @@
     <t>process(clk,rst)begin if rst='1'then slave_out&lt;='0';elsif rising_edge(clk)then slave_out&lt;=not slave_out;end if;end process;</t>
   </si>
   <si>
+    <t>Non gestisce il protocollo SPI, dunque non è uno slave SPI</t>
+  </si>
+  <si>
     <t>Implement a frequency counter using a process.</t>
   </si>
   <si>
@@ -1710,6 +1752,9 @@
     <t>process(clk,rst)begin if rst='1'then count&lt;=0;elsif rising_edge(clk)then count&lt;=count+1;end if;end process;</t>
   </si>
   <si>
+    <t>Senza segnali di enable, ma conta la frequenza</t>
+  </si>
+  <si>
     <t>Write a parallel to serial converter of N-bit with the signals clk, parallel_in (N-bit), and load_en as input and the signal serial_out as output.</t>
   </si>
   <si>
@@ -1719,6 +1764,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity ParallelToSerialConverter is Generic(N : natural := 8); Port ( Clk : in STD_LOGIC; Parallel_In : in STD_LOGIC_VECTOR (N-1 downto 0); Load_En : in STD_LOGIC; Serial_Out : out STD_LOGIC); end ParallelToSerialConverter; architecture Behavioral of ParallelToSerialConverter is begin process (Clk, Load_En) variable temp : STD_LOGIC_VECTOR (N-1 downto 0); begin if (rising_edge(Clk)) then temp := Parallel_In; if (Load_En = '1') then temp := temp(N-2 downto 0) &amp; temp(N-1); end if ; end if ; Serial_Out &lt;= temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Una un singolo bit in output, mi può aandre anche bene con p-s</t>
+  </si>
+  <si>
     <t>Define a fixed-point converter of M-bit with the signal float_value (M-bit) as input and the signal fixed_point (N-bit) as output.</t>
   </si>
   <si>
@@ -1728,6 +1776,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity fixed_point_converter is Generic ( M : natural := 8; N : natural := 8 ); Port ( float_value : in signed(M-1 downto 0); fixed_point : out signed(N-1 downto 0)); end fixed_point_converter; architecture Behavioral of fixed_point_converter is begin process (float_value) variable temp : signed(N-1 downto 0); begin temp := float_value; for i in 0 to M-1 loop if temp(i) = '1' then fixed_point &lt;= temp(i); end if ; end loop ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Sbagliata come conversione</t>
+  </si>
+  <si>
     <t>Create a basic memory controller with read and write operations</t>
   </si>
   <si>
@@ -1737,6 +1788,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then memory_out &lt;= (others =&gt; '0'); elsif read = '1' then memory_out &lt;= memory_in; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non a la write</t>
+  </si>
+  <si>
     <t>Define a frequency divider with the signals clock, reset, and divide_ratio (N-bit) as input and the signal divided_clock as output.</t>
   </si>
   <si>
@@ -1746,6 +1800,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity FrequencyDivider is Generic ( N : natural := 8 ); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Divide_Ratio : in STD_LOGIC_VECTOR (N-1 downto 0); Divided_Clock : out STD_LOGIC); end FrequencyDivider; architecture Behavioral of FrequencyDivider is signal count : unsigned(N-1 downto 0) := (others =&gt; '0'); begin process (Clock, Reset) begin if Reset = '1' then count &lt;= (others =&gt; '0'); elsif rising_edge(Clock) then count &lt;= count + 1; end if ; Divided_Clock &lt;= std_logic_vector(count); end process ; end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Non fa un divisore di frequenza </t>
+  </si>
+  <si>
     <t>Create a basic SPI (Serial Peripheral Interface) master with multiple slave select</t>
   </si>
   <si>
@@ -1755,6 +1812,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then spi_out &lt;= '0'; elsif spi_in = '1' then spi_out &lt;= '1'; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non fa lo slav select come richiesto</t>
+  </si>
+  <si>
     <t>Create a basic PWM (Pulse Width Modulation) generator with variable frequency</t>
   </si>
   <si>
@@ -1773,6 +1833,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity crc_checker is Generic (N : natural := 8; M : natural := 8); Port ( Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Received_CRC : in STD_LOGIC_VECTOR (M-1 downto 0); Polynomial : in STD_LOGIC_VECTOR (M-1 downto 0); CRC_Match : out STD_LOGIC); end crc_checker; architecture Behavioral of crc_checker is begin process (Data_In, Received_CRC, Polynomial) variable crc : unsigned(M-1 downto 0); begin for i in 0 to N-1 loop if (Data_In(i) = '1') then crc := crc + (unsigned(Polynomial) xor crc(i)) &amp; (unsigned(crc(i))); end if ; end loop ; CRC_Match &lt;= crc; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un checker CRC</t>
+  </si>
+  <si>
     <t>Define a fixed-point divider of N-bit with the signals dividend (N-bit) and divisor (N-bit) as input and the signals quotient (N-bit) and remainder (N-bit) as output.</t>
   </si>
   <si>
@@ -1782,6 +1845,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity fixed_point_divider is Generic ( N : natural := 8 ); Port ( dividend : in signed(N-1 downto 0); divisor : in signed(N-1 downto 0); quotient : out signed(N-1 downto 0); remainder : out signed(N-1 downto 0) ); end fixed_point_divider; architecture Behavioral of fixed_point_divider is begin process (dividend, divisor) variable temp_quotient : signed(N-1 downto 0); variable temp_remainder : signed(N-1 downto 0); begin temp_quotient := (others =&gt; '0'); temp_remainder := dividend; for i in 0 to N-1 loop if temp_remainder &gt;= divisor then temp_remainder := temp_remainder - divisor; temp_quotient(i) := '1'; end if ; end loop ; quotient &lt;= temp_quotient; remainder &lt;= temp_remainder; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Equivalente anche se non compre la divisione per zero</t>
+  </si>
+  <si>
     <t>Write a 2-bit magnitude comparator with the signals A1, A0, B1, and B0 as input and the signals A_greater, A_equal, and A_smaller as output.</t>
   </si>
   <si>
@@ -1791,6 +1857,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity magnitude_comparator is Port ( A1 : in STD_LOGIC; A0 : in STD_LOGIC; B1 : in STD_LOGIC; B0 : in STD_LOGIC; A_greater : out STD_LOGIC; A_equal : out STD_LOGIC; A_smaller : out STD_LOGIC); end magnitude_comparator; architecture Behavioral of magnitude_comparator is begin process (A1, A0, B1, B0) variable temp : STD_LOGIC := '0'; begin temp := A1 &amp; A0; if temp = '1' then A_greater &lt;= '1'; A_equal &lt;= '1'; A_smaller &lt;= '0'; elsif temp = '0' then A_greater &lt;= '0'; A_equal &lt;= '0'; A_smaller &lt;= '1'; elsif temp = '1' then A_greater &lt;= '0'; A_equal &lt;= '0'; A_smaller &lt;= '0'; elsif temp = '0' then A_greater &lt;= '0'; A_equal &lt;= '0'; A_smaller &lt;= '1'; elsif temp = '1' then A_greater &lt;= '0'; A_equal &lt;= '1'; A_smaller &lt;= '0'; elsif temp = '0' then A_greater &lt;= '0'; A_equal &lt;= '0'; A_smaller &lt;= '1'; else A_greater &lt;= '0'; A_equal &lt;= '0'; A_smaller &lt;= '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un comparatore di magnitudo</t>
+  </si>
+  <si>
     <t>Write a binary to gray converter of N-bit with the signal binary (N-bit) as input and the signal gray_code (N-bit) as output.</t>
   </si>
   <si>
@@ -1800,6 +1869,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity binary_to_gray is Generic (N : natural := 8); Port ( Binary : in STD_LOGIC_VECTOR (N-1 downto 0); Gray_Code : out STD_LOGIC_VECTOR (N-1 downto 0)); end binary_to_gray; architecture Behavioral of binary_to_gray is begin process (Binary) variable gray_code : std_logic_vector(N-1 downto 0); begin gray_code := Binary; for i in 0 to N-1 loop if gray_code(i) = '1' then gray_code(i) &lt;= '0'; end if ; end loop ; Gray_Code &lt;= gray_code; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un convertitore gray</t>
+  </si>
+  <si>
     <t>Implement a basic quadrature encoder interface</t>
   </si>
   <si>
@@ -1809,6 +1881,9 @@
     <t>entity quadrature_encoder is port (clk : in std_logic; rst : in std_logic; q : out std_logic_vector(7 downto 0)); end entity; architecture Behavioral of quadrature_encoder is signal count : std_logic_vector(7 downto 0) := (others =&gt; '0'); begin process (clk, rst) begin if rst = '1' then count &lt;= (others =&gt; '0'); elsif rising_edge(clk) then count &lt;= count + 1; end if; q &lt;= count; end process; end architecture;</t>
   </si>
   <si>
+    <t>Semplice contatore</t>
+  </si>
+  <si>
     <t>Define a debouncer with the signal noisy_button as input and the signal clean_button_pulse as output.</t>
   </si>
   <si>
@@ -1818,6 +1893,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity debouncer is Port ( Noisy_Button : in STD_LOGIC; Clean_Button_Pulse : out STD_LOGIC); end debouncer; architecture Behavioral of debouncer is begin process (Noisy_Button) variable temp : STD_LOGIC := '0'; begin temp := Noisy_Button; if temp = '1' then Clean_Button_Pulse &lt;= '1'; elsif temp = '0' then Clean_Button_Pulse &lt;= '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non gestirsce il jitter e dunque non è un debouncer</t>
+  </si>
+  <si>
     <t>Define a Johnson ring counter of N-bit with the signals clock and reset as input and the signal count (N-bit) as output.</t>
   </si>
   <si>
@@ -1836,6 +1914,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity pulse_generator is Generic ( N : natural := 8 ); Port ( Clk : in STD_LOGIC; Reset : in STD_LOGIC; Pulse_Width : in STD_LOGIC_VECTOR (N-1 downto 0); Pulse_Out : out STD_LOGIC ); end pulse_generator; architecture Behavioral of pulse_generator is begin process (Clk, Reset) variable counter : integer range 0 to N-1 := 0; begin if (Reset = '1') then counter := 0; elsif (rising_edge(Clk)) then counter := counter + 1; if (counter = Pulse_Width) then Pulse_Out &lt;= '1'; else Pulse_Out &lt;= '0'; end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Equivalenti</t>
+  </si>
+  <si>
     <t>Define a magnitude comparator of K-bit with the signals A (K-bit) and B (K-bit) as input and the signals A_GT_B, A_EQ_B, and A_LT_B as output.</t>
   </si>
   <si>
@@ -1845,6 +1926,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity magnitude_comparator is Generic ( K : natural := 8 ); Port ( A : in STD_LOGIC_VECTOR (K-1 downto 0); B : in STD_LOGIC_VECTOR (K-1 downto 0); A_GT_B : out STD_LOGIC; A_EQ_B : out STD_LOGIC; A_LT_B : out STD_LOGIC ); end magnitude_comparator; architecture Behavioral of magnitude_comparator is begin process (A, B) variable temp : STD_LOGIC_VECTOR (K-1 downto 0); begin temp := A &amp; B; A_GT_B &lt;= temp(K-1 downto 0); A_EQ_B &lt;= temp(K-2 downto 0); A_LT_B &lt;= temp(K-1 downto 0); end process ; end Behavioral;</t>
   </si>
   <si>
+    <t xml:space="preserve">Qualche errore logico però grossomodo va bene </t>
+  </si>
+  <si>
     <t>Define a pseudo-random number generator of N-bit with the signals clock and seed_value (N-bit) as input and the signal random_number (N-bit) as output.</t>
   </si>
   <si>
@@ -1854,6 +1938,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity PRNG is Generic(N : natural := 8); Port ( Clock : in STD_LOGIC; Seed_Value : in STD_LOGIC_VECTOR (N-1 downto 0); Random_Number : out STD_LOGIC_VECTOR (N-1 downto 0)); end PRNG; architecture Behavioral of PRNG is begin process (Clock) variable seed : integer range 0 to N-1 := 0; begin if rising_edge(Clock) then seed := Seed_Value; Random_Number &lt;= seed; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non genera numeri casuali</t>
+  </si>
+  <si>
     <t>Create a configurable clock divider</t>
   </si>
   <si>
@@ -1872,6 +1959,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity AstableMultivibrator is Port ( Clk : in STD_LOGIC; Reset : in STD_LOGIC; Oscillating_Out : out STD_LOGIC); end AstableMultivibrator; architecture Behavioral of AstableMultivibrator is begin process (Clk, Reset) variable temp : STD_LOGIC := '0'; begin if (Reset = '1') then temp := '0'; elsif (rising_edge(Clk)) then temp := temp + 1; end if ; Oscillating_Out &lt;= temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Deve essere fatto qualche cambiamento ma va bene</t>
+  </si>
+  <si>
     <t>Define a rotating priority encoder with the signal request (N-bit) as input and the signals grant (log2N-bit), valid, and rotation_bit as output.</t>
   </si>
   <si>
@@ -1899,6 +1989,9 @@
     <t>entity digital_comparator is port (clk : in std_logic; rst : in std_logic; input : in std_logic_vector(3 downto 0); output : out std_logic_vector(3 downto 0)); end entity; architecture Behavioral of digital_comparator is signal count : std_logic_vector(3 downto 0) := (others =&gt; '0'); begin process (clk, rst) begin if rst = '1' then count &lt;= (others =&gt; '0'); elsif rising_edge(clk) then if input = '1' then count &lt;= count + 1; end if; end if; end process; output &lt;= count; end architecture;</t>
   </si>
   <si>
+    <t>Non è un comparatore</t>
+  </si>
+  <si>
     <t>Define a 2-to-1 multiplexer with the signals data0, data1, and select as input and the signal data_out as output.</t>
   </si>
   <si>
@@ -1917,6 +2010,9 @@
     <t>process(clk,rst)begin if rst='1'then spi_out&lt;='0';elsif rising_edge(clk)then spi_out&lt;=not spi_out;end if;end process;</t>
   </si>
   <si>
+    <t>Non è un SPI master</t>
+  </si>
+  <si>
     <t>Detect falling edge of a signal using a process.</t>
   </si>
   <si>
@@ -1933,6 +2029,9 @@
   </si>
   <si>
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; use IEEE.NUMERIC_STD.ALL; entity universal_shift_register is Generic( P : natural := 8 ); Port ( Clock : in STD_LOGIC; Shift_Enable : in STD_LOGIC; Shift_Direction : in STD_LOGIC; Serial_In : in STD_LOGIC; Parallel_Out : out STD_LOGIC_VECTOR (P-1 downto 0); Serial_Out : out STD_LOGIC ); end universal_shift_register; architecture Behavioral of universal_shift_register is begin process (Clock, Shift_Enable, Shift_Direction, Serial_In) variable temp : STD_LOGIC_VECTOR (P-1 downto 0); begin if rising_edge(Clock) then if Shift_Enable = '1' then temp := Serial_In; elsif Shift_Direction = '0' then temp := temp(P-2 downto 0) &amp; temp(P-1); end if ; end if ; Parallel_Out &lt;= temp; Serial_Out &lt;= temp; end process ; end Behavioral;</t>
+  </si>
+  <si>
+    <t>Apparte qualche errore abbastanza coerenti</t>
   </si>
   <si>
     <t>Implement a basic priority encoder</t>
@@ -2909,8 +3008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="G197" sqref="G197"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="G255" sqref="G255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7522,7 +7621,7 @@
         <v>0.99999451303155007</v>
       </c>
       <c r="G197">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -7570,16 +7669,19 @@
       <c r="G199">
         <v>0</v>
       </c>
+      <c r="H199" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="200" spans="1:8">
       <c r="A200" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B200" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C200" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -7593,16 +7695,19 @@
       <c r="G200">
         <v>0</v>
       </c>
+      <c r="H200" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B201" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C201" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -7616,16 +7721,19 @@
       <c r="G201">
         <v>0</v>
       </c>
+      <c r="H201" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="202" spans="1:8">
       <c r="A202" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="B202" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C202" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -7639,16 +7747,19 @@
       <c r="G202">
         <v>0</v>
       </c>
+      <c r="H202" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="203" spans="1:8">
       <c r="A203" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="B203" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C203" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -7662,16 +7773,19 @@
       <c r="G203">
         <v>0</v>
       </c>
+      <c r="H203" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="204" spans="1:8">
       <c r="A204" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="B204" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="C204" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -7683,18 +7797,18 @@
         <v>0.920940170940171</v>
       </c>
       <c r="G204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:8">
       <c r="A205" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="B205" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="C205" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -7708,16 +7822,19 @@
       <c r="G205">
         <v>0</v>
       </c>
+      <c r="H205" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="206" spans="1:8">
       <c r="A206" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="B206" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="C206" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -7729,18 +7846,18 @@
         <v>0.96282844754104435</v>
       </c>
       <c r="G206">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:8">
       <c r="A207" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="B207" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="C207" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -7752,18 +7869,18 @@
         <v>0.96282844754104435</v>
       </c>
       <c r="G207">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208" spans="1:8">
       <c r="A208" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B208" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="C208" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="D208">
         <v>1</v>
@@ -7778,15 +7895,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:8">
       <c r="A209" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="B209" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="C209" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -7800,16 +7917,19 @@
       <c r="G209">
         <v>0</v>
       </c>
-    </row>
-    <row r="210" spans="1:7">
+      <c r="H209" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8">
       <c r="A210" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="B210" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="C210" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="D210">
         <v>0</v>
@@ -7823,16 +7943,19 @@
       <c r="G210">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:7">
+      <c r="H210" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8">
       <c r="A211" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="B211" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="C211" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -7847,15 +7970,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:8">
       <c r="A212" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="B212" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="C212" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="D212">
         <v>1</v>
@@ -7870,15 +7993,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:8">
       <c r="A213" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="B213" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="C213" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -7890,18 +8013,21 @@
         <v>0.67201737656283123</v>
       </c>
       <c r="G213">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H213" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8">
       <c r="A214" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="B214" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="C214" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="D214">
         <v>1</v>
@@ -7916,15 +8042,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:8">
       <c r="A215" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="B215" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="C215" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="D215">
         <v>1</v>
@@ -7939,15 +8065,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:8">
       <c r="A216" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="B216" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="C216" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -7962,15 +8088,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:8">
       <c r="A217" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="B217" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="C217" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="D217">
         <v>1</v>
@@ -7985,15 +8111,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:8">
       <c r="A218" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="B218" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="C218" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -8008,15 +8134,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:8">
       <c r="A219" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="B219" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="C219" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -8031,15 +8157,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:8">
       <c r="A220" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="B220" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="C220" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -8054,15 +8180,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:8">
       <c r="A221" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="B221" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="C221" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="D221">
         <v>1</v>
@@ -8077,15 +8203,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:7">
+    <row r="222" spans="1:8">
       <c r="A222" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="B222" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="C222" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="D222">
         <v>1</v>
@@ -8100,15 +8226,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:8">
       <c r="A223" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="B223" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="C223" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="D223">
         <v>1</v>
@@ -8123,15 +8249,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:8">
       <c r="A224" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="B224" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="C224" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="D224">
         <v>0</v>
@@ -8145,16 +8271,19 @@
       <c r="G224">
         <v>0</v>
       </c>
-    </row>
-    <row r="225" spans="1:7">
+      <c r="H224" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8">
       <c r="A225" t="s">
-        <v>541</v>
+        <v>550</v>
       </c>
       <c r="B225" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="C225" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
       <c r="D225">
         <v>0</v>
@@ -8168,16 +8297,19 @@
       <c r="G225">
         <v>0</v>
       </c>
-    </row>
-    <row r="226" spans="1:7">
+      <c r="H225" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8">
       <c r="A226" t="s">
-        <v>544</v>
+        <v>554</v>
       </c>
       <c r="B226" t="s">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="C226" t="s">
-        <v>546</v>
+        <v>556</v>
       </c>
       <c r="D226">
         <v>0</v>
@@ -8191,16 +8323,19 @@
       <c r="G226">
         <v>0</v>
       </c>
-    </row>
-    <row r="227" spans="1:7">
+      <c r="H226" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8">
       <c r="A227" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="B227" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="C227" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="D227">
         <v>0</v>
@@ -8212,18 +8347,21 @@
         <v>0.72736625514403297</v>
       </c>
       <c r="G227">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H227" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8">
       <c r="A228" t="s">
-        <v>550</v>
+        <v>562</v>
       </c>
       <c r="B228" t="s">
-        <v>551</v>
+        <v>563</v>
       </c>
       <c r="C228" t="s">
-        <v>552</v>
+        <v>564</v>
       </c>
       <c r="D228">
         <v>0</v>
@@ -8237,16 +8375,19 @@
       <c r="G228">
         <v>0</v>
       </c>
-    </row>
-    <row r="229" spans="1:7">
+      <c r="H228" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8">
       <c r="A229" t="s">
-        <v>553</v>
+        <v>566</v>
       </c>
       <c r="B229" t="s">
-        <v>554</v>
+        <v>567</v>
       </c>
       <c r="C229" t="s">
-        <v>555</v>
+        <v>568</v>
       </c>
       <c r="D229">
         <v>0</v>
@@ -8260,16 +8401,19 @@
       <c r="G229">
         <v>0</v>
       </c>
-    </row>
-    <row r="230" spans="1:7">
+      <c r="H229" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8">
       <c r="A230" t="s">
-        <v>556</v>
+        <v>570</v>
       </c>
       <c r="B230" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
       <c r="C230" t="s">
-        <v>558</v>
+        <v>572</v>
       </c>
       <c r="D230">
         <v>0</v>
@@ -8281,18 +8425,21 @@
         <v>0.62203487013952297</v>
       </c>
       <c r="G230">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="231" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H230" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8">
       <c r="A231" t="s">
-        <v>559</v>
+        <v>574</v>
       </c>
       <c r="B231" t="s">
-        <v>560</v>
+        <v>575</v>
       </c>
       <c r="C231" t="s">
-        <v>561</v>
+        <v>576</v>
       </c>
       <c r="D231">
         <v>0</v>
@@ -8304,18 +8451,21 @@
         <v>0.70559418290806941</v>
       </c>
       <c r="G231">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H231" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8">
       <c r="A232" t="s">
-        <v>562</v>
+        <v>578</v>
       </c>
       <c r="B232" t="s">
-        <v>563</v>
+        <v>579</v>
       </c>
       <c r="C232" t="s">
-        <v>564</v>
+        <v>580</v>
       </c>
       <c r="D232">
         <v>0</v>
@@ -8329,16 +8479,19 @@
       <c r="G232">
         <v>0</v>
       </c>
-    </row>
-    <row r="233" spans="1:7">
+      <c r="H232" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8">
       <c r="A233" t="s">
-        <v>565</v>
+        <v>582</v>
       </c>
       <c r="B233" t="s">
-        <v>566</v>
+        <v>583</v>
       </c>
       <c r="C233" t="s">
-        <v>567</v>
+        <v>584</v>
       </c>
       <c r="D233">
         <v>0</v>
@@ -8352,16 +8505,19 @@
       <c r="G233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:7">
+      <c r="H233" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8">
       <c r="A234" t="s">
-        <v>568</v>
+        <v>586</v>
       </c>
       <c r="B234" t="s">
-        <v>569</v>
+        <v>587</v>
       </c>
       <c r="C234" t="s">
-        <v>570</v>
+        <v>588</v>
       </c>
       <c r="D234">
         <v>0</v>
@@ -8375,16 +8531,19 @@
       <c r="G234">
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:7">
+      <c r="H234" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8">
       <c r="A235" t="s">
-        <v>571</v>
+        <v>590</v>
       </c>
       <c r="B235" t="s">
-        <v>572</v>
+        <v>591</v>
       </c>
       <c r="C235" t="s">
-        <v>573</v>
+        <v>592</v>
       </c>
       <c r="D235">
         <v>0</v>
@@ -8398,16 +8557,19 @@
       <c r="G235">
         <v>0</v>
       </c>
-    </row>
-    <row r="236" spans="1:7">
+      <c r="H235" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8">
       <c r="A236" t="s">
-        <v>574</v>
+        <v>594</v>
       </c>
       <c r="B236" t="s">
-        <v>575</v>
+        <v>595</v>
       </c>
       <c r="C236" t="s">
-        <v>576</v>
+        <v>596</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -8419,18 +8581,21 @@
         <v>0.69291232343846532</v>
       </c>
       <c r="G236">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H236" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8">
       <c r="A237" t="s">
-        <v>577</v>
+        <v>597</v>
       </c>
       <c r="B237" t="s">
-        <v>578</v>
+        <v>598</v>
       </c>
       <c r="C237" t="s">
-        <v>579</v>
+        <v>599</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -8444,16 +8609,19 @@
       <c r="G237">
         <v>0</v>
       </c>
-    </row>
-    <row r="238" spans="1:7">
+      <c r="H237" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8">
       <c r="A238" t="s">
-        <v>580</v>
+        <v>601</v>
       </c>
       <c r="B238" t="s">
-        <v>581</v>
+        <v>602</v>
       </c>
       <c r="C238" t="s">
-        <v>582</v>
+        <v>603</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -8465,18 +8633,21 @@
         <v>0.61077903654581056</v>
       </c>
       <c r="G238">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H238" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8">
       <c r="A239" t="s">
-        <v>583</v>
+        <v>605</v>
       </c>
       <c r="B239" t="s">
-        <v>584</v>
+        <v>606</v>
       </c>
       <c r="C239" t="s">
-        <v>585</v>
+        <v>607</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -8490,16 +8661,19 @@
       <c r="G239">
         <v>0</v>
       </c>
-    </row>
-    <row r="240" spans="1:7">
+      <c r="H239" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8">
       <c r="A240" t="s">
-        <v>586</v>
+        <v>609</v>
       </c>
       <c r="B240" t="s">
-        <v>587</v>
+        <v>610</v>
       </c>
       <c r="C240" t="s">
-        <v>588</v>
+        <v>611</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -8513,16 +8687,19 @@
       <c r="G240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:7">
+      <c r="H240" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
       <c r="A241" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="B241" t="s">
-        <v>590</v>
+        <v>614</v>
       </c>
       <c r="C241" t="s">
-        <v>591</v>
+        <v>615</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -8536,16 +8713,19 @@
       <c r="G241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:7">
+      <c r="H241" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
       <c r="A242" t="s">
-        <v>592</v>
+        <v>617</v>
       </c>
       <c r="B242" t="s">
-        <v>593</v>
+        <v>618</v>
       </c>
       <c r="C242" t="s">
-        <v>594</v>
+        <v>619</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -8559,16 +8739,19 @@
       <c r="G242">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:7">
+      <c r="H242" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
       <c r="A243" t="s">
-        <v>595</v>
+        <v>621</v>
       </c>
       <c r="B243" t="s">
-        <v>596</v>
+        <v>622</v>
       </c>
       <c r="C243" t="s">
-        <v>597</v>
+        <v>623</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -8580,18 +8763,18 @@
         <v>0.82660034438801444</v>
       </c>
       <c r="G243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
       <c r="A244" t="s">
-        <v>598</v>
+        <v>624</v>
       </c>
       <c r="B244" t="s">
-        <v>599</v>
+        <v>625</v>
       </c>
       <c r="C244" t="s">
-        <v>600</v>
+        <v>626</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -8603,18 +8786,21 @@
         <v>0.69100597488726778</v>
       </c>
       <c r="G244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H244" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8">
       <c r="A245" t="s">
-        <v>601</v>
+        <v>628</v>
       </c>
       <c r="B245" t="s">
-        <v>602</v>
+        <v>629</v>
       </c>
       <c r="C245" t="s">
-        <v>603</v>
+        <v>630</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -8626,18 +8812,21 @@
         <v>0.51538467879942984</v>
       </c>
       <c r="G245">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H245" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8">
       <c r="A246" t="s">
-        <v>604</v>
+        <v>632</v>
       </c>
       <c r="B246" t="s">
-        <v>605</v>
+        <v>633</v>
       </c>
       <c r="C246" t="s">
-        <v>606</v>
+        <v>634</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -8651,16 +8840,19 @@
       <c r="G246">
         <v>0</v>
       </c>
-    </row>
-    <row r="247" spans="1:7">
+      <c r="H246" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8">
       <c r="A247" t="s">
-        <v>607</v>
+        <v>636</v>
       </c>
       <c r="B247" t="s">
-        <v>608</v>
+        <v>637</v>
       </c>
       <c r="C247" t="s">
-        <v>609</v>
+        <v>638</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -8672,18 +8864,18 @@
         <v>0.84480070498915405</v>
       </c>
       <c r="G247">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8">
       <c r="A248" t="s">
-        <v>610</v>
+        <v>639</v>
       </c>
       <c r="B248" t="s">
-        <v>611</v>
+        <v>640</v>
       </c>
       <c r="C248" t="s">
-        <v>612</v>
+        <v>641</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -8695,18 +8887,21 @@
         <v>0.90539714212152411</v>
       </c>
       <c r="G248">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H248" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8">
       <c r="A249" t="s">
-        <v>613</v>
+        <v>643</v>
       </c>
       <c r="B249" t="s">
-        <v>614</v>
+        <v>644</v>
       </c>
       <c r="C249" t="s">
-        <v>615</v>
+        <v>645</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -8718,18 +8913,18 @@
         <v>0.65281428171841693</v>
       </c>
       <c r="G249">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8">
       <c r="A250" t="s">
-        <v>616</v>
+        <v>646</v>
       </c>
       <c r="B250" t="s">
-        <v>617</v>
+        <v>647</v>
       </c>
       <c r="C250" t="s">
-        <v>618</v>
+        <v>648</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -8741,18 +8936,18 @@
         <v>0.59366365984966929</v>
       </c>
       <c r="G250">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8">
       <c r="A251" t="s">
-        <v>619</v>
+        <v>649</v>
       </c>
       <c r="B251" t="s">
-        <v>620</v>
+        <v>650</v>
       </c>
       <c r="C251" t="s">
-        <v>621</v>
+        <v>651</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -8766,16 +8961,19 @@
       <c r="G251">
         <v>0</v>
       </c>
-    </row>
-    <row r="252" spans="1:7">
+      <c r="H251" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8">
       <c r="A252" t="s">
-        <v>622</v>
+        <v>653</v>
       </c>
       <c r="B252" t="s">
-        <v>623</v>
+        <v>654</v>
       </c>
       <c r="C252" t="s">
-        <v>624</v>
+        <v>655</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -8787,18 +8985,18 @@
         <v>0.66869639457323349</v>
       </c>
       <c r="G252">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8">
       <c r="A253" t="s">
-        <v>625</v>
+        <v>656</v>
       </c>
       <c r="B253" t="s">
-        <v>626</v>
+        <v>657</v>
       </c>
       <c r="C253" t="s">
-        <v>627</v>
+        <v>658</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -8812,16 +9010,19 @@
       <c r="G253">
         <v>0</v>
       </c>
-    </row>
-    <row r="254" spans="1:7">
+      <c r="H253" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8">
       <c r="A254" t="s">
-        <v>628</v>
+        <v>660</v>
       </c>
       <c r="B254" t="s">
-        <v>629</v>
+        <v>661</v>
       </c>
       <c r="C254" t="s">
-        <v>630</v>
+        <v>662</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -8833,18 +9034,21 @@
         <v>0.65411379743941467</v>
       </c>
       <c r="G254">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H254" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8">
       <c r="A255" t="s">
-        <v>631</v>
+        <v>663</v>
       </c>
       <c r="B255" t="s">
-        <v>632</v>
+        <v>664</v>
       </c>
       <c r="C255" t="s">
-        <v>633</v>
+        <v>665</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -8856,18 +9060,21 @@
         <v>0.70199221052631566</v>
       </c>
       <c r="G255">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H255" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8">
       <c r="A256" t="s">
-        <v>634</v>
+        <v>667</v>
       </c>
       <c r="B256" t="s">
-        <v>635</v>
+        <v>668</v>
       </c>
       <c r="C256" t="s">
-        <v>636</v>
+        <v>669</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -8884,13 +9091,13 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257" t="s">
-        <v>637</v>
+        <v>670</v>
       </c>
       <c r="B257" t="s">
-        <v>638</v>
+        <v>671</v>
       </c>
       <c r="C257" t="s">
-        <v>639</v>
+        <v>672</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -8907,13 +9114,13 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258" t="s">
-        <v>640</v>
+        <v>673</v>
       </c>
       <c r="B258" t="s">
-        <v>641</v>
+        <v>674</v>
       </c>
       <c r="C258" t="s">
-        <v>642</v>
+        <v>675</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -8930,13 +9137,13 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259" t="s">
-        <v>643</v>
+        <v>676</v>
       </c>
       <c r="B259" t="s">
-        <v>644</v>
+        <v>677</v>
       </c>
       <c r="C259" t="s">
-        <v>645</v>
+        <v>678</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -8953,13 +9160,13 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260" t="s">
-        <v>646</v>
+        <v>679</v>
       </c>
       <c r="B260" t="s">
-        <v>647</v>
+        <v>680</v>
       </c>
       <c r="C260" t="s">
-        <v>648</v>
+        <v>681</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -8976,13 +9183,13 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" t="s">
-        <v>649</v>
+        <v>682</v>
       </c>
       <c r="B261" t="s">
-        <v>650</v>
+        <v>683</v>
       </c>
       <c r="C261" t="s">
-        <v>651</v>
+        <v>684</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -8999,13 +9206,13 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262" t="s">
-        <v>652</v>
+        <v>685</v>
       </c>
       <c r="B262" t="s">
-        <v>653</v>
+        <v>686</v>
       </c>
       <c r="C262" t="s">
-        <v>654</v>
+        <v>687</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -9022,13 +9229,13 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263" t="s">
-        <v>655</v>
+        <v>688</v>
       </c>
       <c r="B263" t="s">
-        <v>656</v>
+        <v>689</v>
       </c>
       <c r="C263" t="s">
-        <v>657</v>
+        <v>690</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9045,13 +9252,13 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" t="s">
-        <v>658</v>
+        <v>691</v>
       </c>
       <c r="B264" t="s">
-        <v>659</v>
+        <v>692</v>
       </c>
       <c r="C264" t="s">
-        <v>660</v>
+        <v>693</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9068,13 +9275,13 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" t="s">
-        <v>661</v>
+        <v>694</v>
       </c>
       <c r="B265" t="s">
-        <v>662</v>
+        <v>695</v>
       </c>
       <c r="C265" t="s">
-        <v>663</v>
+        <v>696</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9091,13 +9298,13 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" t="s">
-        <v>664</v>
+        <v>697</v>
       </c>
       <c r="B266" t="s">
-        <v>665</v>
+        <v>698</v>
       </c>
       <c r="C266" t="s">
-        <v>666</v>
+        <v>699</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9114,13 +9321,13 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" t="s">
-        <v>667</v>
+        <v>700</v>
       </c>
       <c r="B267" t="s">
-        <v>668</v>
+        <v>701</v>
       </c>
       <c r="C267" t="s">
-        <v>669</v>
+        <v>702</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9137,13 +9344,13 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" t="s">
-        <v>670</v>
+        <v>703</v>
       </c>
       <c r="B268" t="s">
-        <v>671</v>
+        <v>704</v>
       </c>
       <c r="C268" t="s">
-        <v>672</v>
+        <v>705</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9160,13 +9367,13 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" t="s">
-        <v>673</v>
+        <v>706</v>
       </c>
       <c r="B269" t="s">
-        <v>674</v>
+        <v>707</v>
       </c>
       <c r="C269" t="s">
-        <v>675</v>
+        <v>708</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9183,13 +9390,13 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" t="s">
-        <v>676</v>
+        <v>709</v>
       </c>
       <c r="B270" t="s">
-        <v>677</v>
+        <v>710</v>
       </c>
       <c r="C270" t="s">
-        <v>678</v>
+        <v>711</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -9206,13 +9413,13 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" t="s">
-        <v>679</v>
+        <v>712</v>
       </c>
       <c r="B271" t="s">
-        <v>680</v>
+        <v>713</v>
       </c>
       <c r="C271" t="s">
-        <v>681</v>
+        <v>714</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9229,13 +9436,13 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" t="s">
-        <v>682</v>
+        <v>715</v>
       </c>
       <c r="B272" t="s">
-        <v>683</v>
+        <v>716</v>
       </c>
       <c r="C272" t="s">
-        <v>684</v>
+        <v>717</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -9252,13 +9459,13 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" t="s">
-        <v>685</v>
+        <v>718</v>
       </c>
       <c r="B273" t="s">
-        <v>686</v>
+        <v>719</v>
       </c>
       <c r="C273" t="s">
-        <v>687</v>
+        <v>720</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -9275,13 +9482,13 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" t="s">
-        <v>688</v>
+        <v>721</v>
       </c>
       <c r="B274" t="s">
-        <v>689</v>
+        <v>722</v>
       </c>
       <c r="C274" t="s">
-        <v>690</v>
+        <v>723</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -9298,13 +9505,13 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" t="s">
-        <v>691</v>
+        <v>724</v>
       </c>
       <c r="B275" t="s">
-        <v>692</v>
+        <v>725</v>
       </c>
       <c r="C275" t="s">
-        <v>693</v>
+        <v>726</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -9321,13 +9528,13 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" t="s">
-        <v>694</v>
+        <v>727</v>
       </c>
       <c r="B276" t="s">
-        <v>695</v>
+        <v>728</v>
       </c>
       <c r="C276" t="s">
-        <v>696</v>
+        <v>729</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9344,13 +9551,13 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277" t="s">
-        <v>697</v>
+        <v>730</v>
       </c>
       <c r="B277" t="s">
-        <v>698</v>
+        <v>731</v>
       </c>
       <c r="C277" t="s">
-        <v>699</v>
+        <v>732</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -9367,13 +9574,13 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278" t="s">
-        <v>700</v>
+        <v>733</v>
       </c>
       <c r="B278" t="s">
-        <v>701</v>
+        <v>734</v>
       </c>
       <c r="C278" t="s">
-        <v>701</v>
+        <v>734</v>
       </c>
       <c r="D278">
         <v>1</v>
@@ -9390,13 +9597,13 @@
     </row>
     <row r="279" spans="1:7">
       <c r="A279" t="s">
-        <v>702</v>
+        <v>735</v>
       </c>
       <c r="B279" t="s">
-        <v>703</v>
+        <v>736</v>
       </c>
       <c r="C279" t="s">
-        <v>704</v>
+        <v>737</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -9413,13 +9620,13 @@
     </row>
     <row r="280" spans="1:7">
       <c r="A280" t="s">
-        <v>705</v>
+        <v>738</v>
       </c>
       <c r="B280" t="s">
-        <v>706</v>
+        <v>739</v>
       </c>
       <c r="C280" t="s">
-        <v>707</v>
+        <v>740</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -9436,13 +9643,13 @@
     </row>
     <row r="281" spans="1:7">
       <c r="A281" t="s">
-        <v>708</v>
+        <v>741</v>
       </c>
       <c r="B281" t="s">
-        <v>709</v>
+        <v>742</v>
       </c>
       <c r="C281" t="s">
-        <v>709</v>
+        <v>742</v>
       </c>
       <c r="D281">
         <v>1</v>
@@ -9459,13 +9666,13 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282" t="s">
-        <v>710</v>
+        <v>743</v>
       </c>
       <c r="B282" t="s">
-        <v>711</v>
+        <v>744</v>
       </c>
       <c r="C282" t="s">
-        <v>712</v>
+        <v>745</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -9482,13 +9689,13 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283" t="s">
-        <v>713</v>
+        <v>746</v>
       </c>
       <c r="B283" t="s">
-        <v>714</v>
+        <v>747</v>
       </c>
       <c r="C283" t="s">
-        <v>715</v>
+        <v>748</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -9505,13 +9712,13 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" t="s">
-        <v>716</v>
+        <v>749</v>
       </c>
       <c r="B284" t="s">
-        <v>717</v>
+        <v>750</v>
       </c>
       <c r="C284" t="s">
-        <v>718</v>
+        <v>751</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -9528,13 +9735,13 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" t="s">
-        <v>719</v>
+        <v>752</v>
       </c>
       <c r="B285" t="s">
-        <v>720</v>
+        <v>753</v>
       </c>
       <c r="C285" t="s">
-        <v>721</v>
+        <v>754</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -9551,13 +9758,13 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" t="s">
-        <v>722</v>
+        <v>755</v>
       </c>
       <c r="B286" t="s">
-        <v>723</v>
+        <v>756</v>
       </c>
       <c r="C286" t="s">
-        <v>724</v>
+        <v>757</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -9574,13 +9781,13 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" t="s">
-        <v>725</v>
+        <v>758</v>
       </c>
       <c r="B287" t="s">
-        <v>726</v>
+        <v>759</v>
       </c>
       <c r="C287" t="s">
-        <v>727</v>
+        <v>760</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -9597,13 +9804,13 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" t="s">
-        <v>728</v>
+        <v>761</v>
       </c>
       <c r="B288" t="s">
-        <v>729</v>
+        <v>762</v>
       </c>
       <c r="C288" t="s">
-        <v>730</v>
+        <v>763</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -9620,13 +9827,13 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" t="s">
-        <v>731</v>
+        <v>764</v>
       </c>
       <c r="B289" t="s">
-        <v>732</v>
+        <v>765</v>
       </c>
       <c r="C289" t="s">
-        <v>733</v>
+        <v>766</v>
       </c>
       <c r="D289">
         <v>0</v>
@@ -9643,13 +9850,13 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" t="s">
-        <v>734</v>
+        <v>767</v>
       </c>
       <c r="B290" t="s">
-        <v>735</v>
+        <v>768</v>
       </c>
       <c r="C290" t="s">
-        <v>735</v>
+        <v>768</v>
       </c>
       <c r="D290">
         <v>1</v>
@@ -9666,13 +9873,13 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" t="s">
-        <v>736</v>
+        <v>769</v>
       </c>
       <c r="B291" t="s">
-        <v>737</v>
+        <v>770</v>
       </c>
       <c r="C291" t="s">
-        <v>737</v>
+        <v>770</v>
       </c>
       <c r="D291">
         <v>1</v>
@@ -9689,13 +9896,13 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" t="s">
-        <v>738</v>
+        <v>771</v>
       </c>
       <c r="B292" t="s">
-        <v>739</v>
+        <v>772</v>
       </c>
       <c r="C292" t="s">
-        <v>740</v>
+        <v>773</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -9712,13 +9919,13 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" t="s">
-        <v>741</v>
+        <v>774</v>
       </c>
       <c r="B293" t="s">
-        <v>742</v>
+        <v>775</v>
       </c>
       <c r="C293" t="s">
-        <v>743</v>
+        <v>776</v>
       </c>
       <c r="D293">
         <v>0</v>
@@ -9735,13 +9942,13 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" t="s">
-        <v>744</v>
+        <v>777</v>
       </c>
       <c r="B294" t="s">
-        <v>745</v>
+        <v>778</v>
       </c>
       <c r="C294" t="s">
-        <v>746</v>
+        <v>779</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -9758,13 +9965,13 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" t="s">
-        <v>747</v>
+        <v>780</v>
       </c>
       <c r="B295" t="s">
-        <v>748</v>
+        <v>781</v>
       </c>
       <c r="C295" t="s">
-        <v>749</v>
+        <v>782</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -9781,13 +9988,13 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" t="s">
-        <v>750</v>
+        <v>783</v>
       </c>
       <c r="B296" t="s">
-        <v>751</v>
+        <v>784</v>
       </c>
       <c r="C296" t="s">
-        <v>752</v>
+        <v>785</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -9804,13 +10011,13 @@
     </row>
     <row r="297" spans="1:7">
       <c r="A297" t="s">
-        <v>753</v>
+        <v>786</v>
       </c>
       <c r="B297" t="s">
-        <v>754</v>
+        <v>787</v>
       </c>
       <c r="C297" t="s">
-        <v>754</v>
+        <v>787</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -9827,13 +10034,13 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" t="s">
-        <v>755</v>
+        <v>788</v>
       </c>
       <c r="B298" t="s">
-        <v>756</v>
+        <v>789</v>
       </c>
       <c r="C298" t="s">
-        <v>757</v>
+        <v>790</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -9850,13 +10057,13 @@
     </row>
     <row r="299" spans="1:7">
       <c r="A299" t="s">
-        <v>758</v>
+        <v>791</v>
       </c>
       <c r="B299" t="s">
-        <v>759</v>
+        <v>792</v>
       </c>
       <c r="C299" t="s">
-        <v>759</v>
+        <v>792</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -9873,13 +10080,13 @@
     </row>
     <row r="300" spans="1:7">
       <c r="A300" t="s">
-        <v>760</v>
+        <v>793</v>
       </c>
       <c r="B300" t="s">
-        <v>761</v>
+        <v>794</v>
       </c>
       <c r="C300" t="s">
-        <v>762</v>
+        <v>795</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -9896,13 +10103,13 @@
     </row>
     <row r="301" spans="1:7">
       <c r="A301" t="s">
-        <v>763</v>
+        <v>796</v>
       </c>
       <c r="B301" t="s">
-        <v>764</v>
+        <v>797</v>
       </c>
       <c r="C301" t="s">
-        <v>765</v>
+        <v>798</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -9919,13 +10126,13 @@
     </row>
     <row r="302" spans="1:7">
       <c r="A302" t="s">
-        <v>766</v>
+        <v>799</v>
       </c>
       <c r="B302" t="s">
-        <v>767</v>
+        <v>800</v>
       </c>
       <c r="C302" t="s">
-        <v>768</v>
+        <v>801</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -9942,13 +10149,13 @@
     </row>
     <row r="303" spans="1:7">
       <c r="A303" t="s">
-        <v>769</v>
+        <v>802</v>
       </c>
       <c r="B303" t="s">
-        <v>770</v>
+        <v>803</v>
       </c>
       <c r="C303" t="s">
-        <v>771</v>
+        <v>804</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -9965,13 +10172,13 @@
     </row>
     <row r="304" spans="1:7">
       <c r="A304" t="s">
-        <v>772</v>
+        <v>805</v>
       </c>
       <c r="B304" t="s">
-        <v>773</v>
+        <v>806</v>
       </c>
       <c r="C304" t="s">
-        <v>774</v>
+        <v>807</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -9988,13 +10195,13 @@
     </row>
     <row r="305" spans="1:7">
       <c r="A305" t="s">
-        <v>775</v>
+        <v>808</v>
       </c>
       <c r="B305" t="s">
-        <v>776</v>
+        <v>809</v>
       </c>
       <c r="C305" t="s">
-        <v>776</v>
+        <v>809</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -10011,13 +10218,13 @@
     </row>
     <row r="306" spans="1:7">
       <c r="A306" t="s">
-        <v>777</v>
+        <v>810</v>
       </c>
       <c r="B306" t="s">
-        <v>778</v>
+        <v>811</v>
       </c>
       <c r="C306" t="s">
-        <v>779</v>
+        <v>812</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10034,13 +10241,13 @@
     </row>
     <row r="307" spans="1:7">
       <c r="A307" t="s">
-        <v>780</v>
+        <v>813</v>
       </c>
       <c r="B307" t="s">
-        <v>781</v>
+        <v>814</v>
       </c>
       <c r="C307" t="s">
-        <v>782</v>
+        <v>815</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10057,13 +10264,13 @@
     </row>
     <row r="308" spans="1:7">
       <c r="A308" t="s">
-        <v>783</v>
+        <v>816</v>
       </c>
       <c r="B308" t="s">
-        <v>784</v>
+        <v>817</v>
       </c>
       <c r="C308" t="s">
-        <v>785</v>
+        <v>818</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10080,13 +10287,13 @@
     </row>
     <row r="309" spans="1:7">
       <c r="A309" t="s">
-        <v>786</v>
+        <v>819</v>
       </c>
       <c r="B309" t="s">
-        <v>787</v>
+        <v>820</v>
       </c>
       <c r="C309" t="s">
-        <v>788</v>
+        <v>821</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10103,13 +10310,13 @@
     </row>
     <row r="310" spans="1:7">
       <c r="A310" t="s">
-        <v>789</v>
+        <v>822</v>
       </c>
       <c r="B310" t="s">
-        <v>790</v>
+        <v>823</v>
       </c>
       <c r="C310" t="s">
-        <v>790</v>
+        <v>823</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -10126,13 +10333,13 @@
     </row>
     <row r="311" spans="1:7">
       <c r="A311" t="s">
-        <v>791</v>
+        <v>824</v>
       </c>
       <c r="B311" t="s">
-        <v>792</v>
+        <v>825</v>
       </c>
       <c r="C311" t="s">
-        <v>793</v>
+        <v>826</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -10149,13 +10356,13 @@
     </row>
     <row r="312" spans="1:7">
       <c r="A312" t="s">
-        <v>794</v>
+        <v>827</v>
       </c>
       <c r="B312" t="s">
-        <v>795</v>
+        <v>828</v>
       </c>
       <c r="C312" t="s">
-        <v>795</v>
+        <v>828</v>
       </c>
       <c r="D312">
         <v>1</v>
@@ -10172,13 +10379,13 @@
     </row>
     <row r="313" spans="1:7">
       <c r="A313" t="s">
-        <v>796</v>
+        <v>829</v>
       </c>
       <c r="B313" t="s">
-        <v>797</v>
+        <v>830</v>
       </c>
       <c r="C313" t="s">
-        <v>798</v>
+        <v>831</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10195,13 +10402,13 @@
     </row>
     <row r="314" spans="1:7">
       <c r="A314" t="s">
-        <v>799</v>
+        <v>832</v>
       </c>
       <c r="B314" t="s">
-        <v>800</v>
+        <v>833</v>
       </c>
       <c r="C314" t="s">
-        <v>801</v>
+        <v>834</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10218,13 +10425,13 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" t="s">
-        <v>802</v>
+        <v>835</v>
       </c>
       <c r="B315" t="s">
-        <v>803</v>
+        <v>836</v>
       </c>
       <c r="C315" t="s">
-        <v>804</v>
+        <v>837</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10241,13 +10448,13 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" t="s">
-        <v>805</v>
+        <v>838</v>
       </c>
       <c r="B316" t="s">
-        <v>806</v>
+        <v>839</v>
       </c>
       <c r="C316" t="s">
-        <v>807</v>
+        <v>840</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10264,13 +10471,13 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" t="s">
-        <v>808</v>
+        <v>841</v>
       </c>
       <c r="B317" t="s">
-        <v>809</v>
+        <v>842</v>
       </c>
       <c r="C317" t="s">
-        <v>809</v>
+        <v>842</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -10287,13 +10494,13 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" t="s">
-        <v>810</v>
+        <v>843</v>
       </c>
       <c r="B318" t="s">
-        <v>811</v>
+        <v>844</v>
       </c>
       <c r="C318" t="s">
-        <v>812</v>
+        <v>845</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10310,13 +10517,13 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" t="s">
-        <v>813</v>
+        <v>846</v>
       </c>
       <c r="B319" t="s">
-        <v>814</v>
+        <v>847</v>
       </c>
       <c r="C319" t="s">
-        <v>815</v>
+        <v>848</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10333,13 +10540,13 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" t="s">
-        <v>816</v>
+        <v>849</v>
       </c>
       <c r="B320" t="s">
-        <v>817</v>
+        <v>850</v>
       </c>
       <c r="C320" t="s">
-        <v>817</v>
+        <v>850</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -10356,13 +10563,13 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>818</v>
+        <v>851</v>
       </c>
       <c r="B321" t="s">
-        <v>819</v>
+        <v>852</v>
       </c>
       <c r="C321" t="s">
-        <v>820</v>
+        <v>853</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -10379,13 +10586,13 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>821</v>
+        <v>854</v>
       </c>
       <c r="B322" t="s">
-        <v>822</v>
+        <v>855</v>
       </c>
       <c r="C322" t="s">
-        <v>823</v>
+        <v>856</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -10402,13 +10609,13 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>824</v>
+        <v>857</v>
       </c>
       <c r="B323" t="s">
-        <v>825</v>
+        <v>858</v>
       </c>
       <c r="C323" t="s">
-        <v>826</v>
+        <v>859</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -10425,13 +10632,13 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>827</v>
+        <v>860</v>
       </c>
       <c r="B324" t="s">
-        <v>828</v>
+        <v>861</v>
       </c>
       <c r="C324" t="s">
-        <v>829</v>
+        <v>862</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10448,13 +10655,13 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>830</v>
+        <v>863</v>
       </c>
       <c r="B325" t="s">
-        <v>831</v>
+        <v>864</v>
       </c>
       <c r="C325" t="s">
-        <v>832</v>
+        <v>865</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10471,13 +10678,13 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>833</v>
+        <v>866</v>
       </c>
       <c r="B326" t="s">
-        <v>834</v>
+        <v>867</v>
       </c>
       <c r="C326" t="s">
-        <v>835</v>
+        <v>868</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -10494,13 +10701,13 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>836</v>
+        <v>869</v>
       </c>
       <c r="B327" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
       <c r="C327" t="s">
-        <v>837</v>
+        <v>870</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>

<commit_message>
Termine analisi CodeT5, aggiunti file di analisi sintetici, aggiustato il framework di analisi
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeT5_225.xlsx
+++ b/HE/W_in_progress/AnalisiCodeT5_225.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A676FA84-8D01-4507-9109-F4AFF7DE81CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34BCF2DF-B0FD-49F5-88FD-CBAEF4D09407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="894">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="904">
   <si>
     <t>IN</t>
   </si>
@@ -2442,6 +2442,9 @@
     <t>stimulus: process begin wait for 100 ns; wait for 10 ns; a&lt;="00"; wait; wait; address(0)&lt;="0";; signal rst_n : std_logic := '1';</t>
   </si>
   <si>
+    <t>Qualche errore sintattico, però va bene</t>
+  </si>
+  <si>
     <t>unita_operativa is a component with X, Y as input std_logic_vectors of 8 bits, clock, reset as input std_logic signals, loadAQ, shift, loadM, sub, selM, selAQ, selF, count_in as input std_logic signals, count as output std_logic_vector of 3 bits, P as output std_logic_vector of 16 bits; set the first bit of signal_19 to signal_20; map signal done_o to the output port t_done</t>
   </si>
   <si>
@@ -2451,6 +2454,9 @@
     <t>component unita_operativa is port( X, Y: in std_logic_vector(7 downto 0); clock, reset: in std_logic; loadAQ, shift, loadM, sub, selM, selAQ, selF, count_in: in std_logic; count: out std_logic_vector(2 downto 0); P: out std_logic_vector(15 downto 0)); end component; signal done_o : std_logic;</t>
   </si>
   <si>
+    <t>Non fa l'ultima operazione</t>
+  </si>
+  <si>
     <t>right shift by 3 bits i_data_1_out and add the value of i_sck_cpy; ROM is a component with RST as input std_logic signal, ADDR as input std_logic_vector signal of 3 bit, DATA as output std_logic_vector signal of 32 bit</t>
   </si>
   <si>
@@ -2517,6 +2523,9 @@
     <t>clk_process : process begin TbClockA &lt;= '0'; count_nxt &lt;= count_reg when enable = '0' else 0 when count_reg = DIV - 1 else count_reg + 1;; component shift_register port (clk : in std_logic; rst : in std_logic; count_reg : in std_logic_vector(2 downto 0); enable : in std_logic; end component;;</t>
   </si>
   <si>
+    <t>Non genera il clock come richiesto</t>
+  </si>
+  <si>
     <t>map data_2_o to t_dac_val_2; if bits 21-14 of BAR signal are equal to hexadecimal '2B'; Use the select statement with GPIO_enable signal to determine whether to output data from GPIO_write signal or keep it high impedance (Z).Report an error message with failure severity if the output signal does not equal '0'</t>
   </si>
   <si>
@@ -2526,6 +2535,9 @@
     <t>data_2_o =&gt; t_dac_val_2; if bar(21 downto 14) = x"2B" then ; end if;; GPIO_enable &lt;= GPIO_write when '0', '1' when others;</t>
   </si>
   <si>
+    <t>Completamente sbagliato</t>
+  </si>
+  <si>
     <t>declare control as a std_logic_vector signal with 2 bit initialized to all '0'; reg_key_in is an input std_logic_vector of 80 bit</t>
   </si>
   <si>
@@ -2541,6 +2553,9 @@
     <t>signal ytemp : std_logic; if abc(18 downto 11) = x"5E" then ; end if;; anodes : out std_logic_vector(7 downto 0);</t>
   </si>
   <si>
+    <t>non digliara il segnale ytemp a 4 bit</t>
+  </si>
+  <si>
     <t>wait for 100 ns, set plaintext to hexadecimal value '0x0000000000000000', and user_key to hexadecimal value '0x00000000000000000000'; unita_controllo is a component with input std_logic signals q0, clock, reset, start and output std_logic signals count of 3 bits, loadM, count_in, loadAQ, en_shift, selM, selAQ, selF, subtract, stop_cu.; c is a constant of type std_logic_vector of 7 bit initialized to '1000110'</t>
   </si>
   <si>
@@ -2607,6 +2622,9 @@
     <t>if ghi(16 downto 9) = x"77" then ; end if; case w is when 'U' =&gt; w := 'X'; when 'X' =&gt; if w2 = '0' then w := 'X'; else w := 'X'; end if; end case;</t>
   </si>
   <si>
+    <t>Inefficiente ma va bene</t>
+  </si>
+  <si>
     <t>ROM_selector_onboard is an entity with clock_in as input std_logic signal, reset_in as input std_logic signal, addr_strobe_in as input std_logic signal, anodes_out as output std_logic_vector signal of 8 bit, cathodes_out as output std_logic_vector signal of 8 bit; temp_stop_cu ia s std_logic signal; define a signal of type std_logic initialized to 0 and called TbClockA</t>
   </si>
   <si>
@@ -2625,6 +2643,9 @@
     <t>entity ripple_carry is port( X, Y: in std_logic_vector(7 downto 0); c_in: in std_logic_vector(7 downto 0); c_out: out std_logic_vector(7 downto 0); Z: out std_logic_vector(7 downto 0)); end ripple_carry; with c.b_request_complete select c.a_request.be &lt;= c.sys_master_ctrl_out.be when '1', r.b_request.be when '0', X when others;</t>
   </si>
   <si>
+    <t>Non dichiara la libreria standard alla fine</t>
+  </si>
+  <si>
     <t>if i_start_counter is lesser to START_DLY minus 1, increase i_start_counter signal by 1, set t_start signal to low; using the selected signal assignment, the signal y is set to a0 when signal ciao is low, it is set to a1 when signal ciao is high, otherwise it is set to don't care</t>
   </si>
   <si>
@@ -2640,6 +2661,9 @@
     <t>clkena &lt;= '1' when clk2xen = 0 else '0'; signal round_key_temp: std_logic_vector(63 downto 0);; component sbox port (); end component;</t>
   </si>
   <si>
+    <t>Non equivalenti per quello che è stato richiesto</t>
+  </si>
+  <si>
     <t>t_stb is a signal of type std_logic; concatenate two 18-bit slices from reg_key_in and two 61-bit slices from reg_key_in, store the result in key_temp1</t>
   </si>
   <si>
@@ -2649,6 +2673,9 @@
     <t>signal t_stb : std_logic; key_temp1 &lt;= reg_key_in(18 downto 0);</t>
   </si>
   <si>
+    <t xml:space="preserve">Noin fa la concatenazione </t>
+  </si>
+  <si>
     <t>set signal result_sig as the XOR of input_x and input_y; i_sck_cpy is a signal of type std_logic; pl is an instance of perm_layer component with the signals data_out_temp2, data_out</t>
   </si>
   <si>
@@ -2707,6 +2734,9 @@
   </si>
   <si>
     <t>i_cs_re_tk &lt;= '1' when i_cs_cpy = '0' and i_cs = '1' else '0'; variable limit : integer range 0 to 255;;</t>
+  </si>
+  <si>
+    <t>Non fa l'inizializzazione come richiesto</t>
   </si>
   <si>
     <t>wait for 10 nanoseconds; cs_o is an output std_logic signal</t>
@@ -3077,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
-      <selection activeCell="I286" sqref="I286"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="H325" sqref="H325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9940,7 +9970,7 @@
         <v>0.9207444976675746</v>
       </c>
       <c r="G287">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288" spans="1:8">
@@ -9963,10 +9993,10 @@
         <v>0.73595387209442364</v>
       </c>
       <c r="G288">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8">
       <c r="A289" t="s">
         <v>787</v>
       </c>
@@ -9986,10 +10016,10 @@
         <v>0.91802796173657109</v>
       </c>
       <c r="G289">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8">
       <c r="A290" t="s">
         <v>790</v>
       </c>
@@ -10012,7 +10042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:8">
       <c r="A291" t="s">
         <v>792</v>
       </c>
@@ -10035,7 +10065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:8">
       <c r="A292" t="s">
         <v>794</v>
       </c>
@@ -10055,10 +10085,10 @@
         <v>0.94878006391408132</v>
       </c>
       <c r="G292">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8">
       <c r="A293" t="s">
         <v>797</v>
       </c>
@@ -10078,10 +10108,10 @@
         <v>0.99610749193911696</v>
       </c>
       <c r="G293">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="294" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8">
       <c r="A294" t="s">
         <v>800</v>
       </c>
@@ -10101,18 +10131,21 @@
         <v>0.81583432485448759</v>
       </c>
       <c r="G294">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="295" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H294" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8">
       <c r="A295" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B295" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C295" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -10126,16 +10159,19 @@
       <c r="G295">
         <v>0</v>
       </c>
-    </row>
-    <row r="296" spans="1:7">
+      <c r="H295" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8">
       <c r="A296" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="B296" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C296" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -10147,18 +10183,18 @@
         <v>0.99999518411142041</v>
       </c>
       <c r="G296">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="297" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8">
       <c r="A297" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B297" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C297" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D297">
         <v>1</v>
@@ -10173,15 +10209,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:8">
       <c r="A298" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B298" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="C298" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -10193,18 +10229,18 @@
         <v>0.87427389227586383</v>
       </c>
       <c r="G298">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8">
       <c r="A299" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B299" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="C299" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D299">
         <v>1</v>
@@ -10219,15 +10255,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:7">
+    <row r="300" spans="1:8">
       <c r="A300" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B300" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C300" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -10239,18 +10275,21 @@
         <v>0.77209302325581408</v>
       </c>
       <c r="G300">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H300" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8">
       <c r="A301" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B301" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="C301" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10262,18 +10301,18 @@
         <v>0.99962434259954924</v>
       </c>
       <c r="G301">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8">
       <c r="A302" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B302" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C302" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -10285,18 +10324,18 @@
         <v>0.999996</v>
       </c>
       <c r="G302">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="303" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8">
       <c r="A303" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B303" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C303" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10310,16 +10349,19 @@
       <c r="G303">
         <v>0</v>
       </c>
-    </row>
-    <row r="304" spans="1:7">
+      <c r="H303" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8">
       <c r="A304" t="s">
-        <v>828</v>
+        <v>831</v>
       </c>
       <c r="B304" t="s">
-        <v>829</v>
+        <v>832</v>
       </c>
       <c r="C304" t="s">
-        <v>830</v>
+        <v>833</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10333,16 +10375,19 @@
       <c r="G304">
         <v>0</v>
       </c>
-    </row>
-    <row r="305" spans="1:7">
+      <c r="H304" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8">
       <c r="A305" t="s">
-        <v>831</v>
+        <v>835</v>
       </c>
       <c r="B305" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
       <c r="C305" t="s">
-        <v>832</v>
+        <v>836</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -10357,15 +10402,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:8">
       <c r="A306" t="s">
-        <v>833</v>
+        <v>837</v>
       </c>
       <c r="B306" t="s">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="C306" t="s">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10379,16 +10424,19 @@
       <c r="G306">
         <v>0</v>
       </c>
-    </row>
-    <row r="307" spans="1:7">
+      <c r="H306" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8">
       <c r="A307" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="B307" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="C307" t="s">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10400,18 +10448,18 @@
         <v>0.952978987738346</v>
       </c>
       <c r="G307">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="308" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8">
       <c r="A308" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="B308" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
       <c r="C308" t="s">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10423,18 +10471,18 @@
         <v>0.98664022774046589</v>
       </c>
       <c r="G308">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="309" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8">
       <c r="A309" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
       <c r="B309" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="C309" t="s">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10446,18 +10494,18 @@
         <v>0.99995890523547304</v>
       </c>
       <c r="G309">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="310" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8">
       <c r="A310" t="s">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="B310" t="s">
-        <v>846</v>
+        <v>851</v>
       </c>
       <c r="C310" t="s">
-        <v>846</v>
+        <v>851</v>
       </c>
       <c r="D310">
         <v>1</v>
@@ -10472,15 +10520,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:8">
       <c r="A311" t="s">
-        <v>847</v>
+        <v>852</v>
       </c>
       <c r="B311" t="s">
-        <v>848</v>
+        <v>853</v>
       </c>
       <c r="C311" t="s">
-        <v>849</v>
+        <v>854</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -10492,18 +10540,18 @@
         <v>0.99998928326474623</v>
       </c>
       <c r="G311">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="312" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8">
       <c r="A312" t="s">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c r="B312" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="C312" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="D312">
         <v>1</v>
@@ -10518,15 +10566,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:7">
+    <row r="313" spans="1:8">
       <c r="A313" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="B313" t="s">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="C313" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10538,18 +10586,18 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8">
       <c r="A314" t="s">
-        <v>855</v>
+        <v>860</v>
       </c>
       <c r="B314" t="s">
-        <v>856</v>
+        <v>861</v>
       </c>
       <c r="C314" t="s">
-        <v>857</v>
+        <v>862</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10561,18 +10609,21 @@
         <v>0.75576340383299623</v>
       </c>
       <c r="G314">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H314" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8">
       <c r="A315" t="s">
-        <v>858</v>
+        <v>864</v>
       </c>
       <c r="B315" t="s">
-        <v>859</v>
+        <v>865</v>
       </c>
       <c r="C315" t="s">
-        <v>860</v>
+        <v>866</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10584,18 +10635,18 @@
         <v>0.99999768518518517</v>
       </c>
       <c r="G315">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8">
       <c r="A316" t="s">
-        <v>861</v>
+        <v>867</v>
       </c>
       <c r="B316" t="s">
-        <v>862</v>
+        <v>868</v>
       </c>
       <c r="C316" t="s">
-        <v>863</v>
+        <v>869</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10609,16 +10660,19 @@
       <c r="G316">
         <v>0</v>
       </c>
-    </row>
-    <row r="317" spans="1:7">
+      <c r="H316" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8">
       <c r="A317" t="s">
-        <v>864</v>
+        <v>871</v>
       </c>
       <c r="B317" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="C317" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="D317">
         <v>1</v>
@@ -10633,15 +10687,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:7">
+    <row r="318" spans="1:8">
       <c r="A318" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="B318" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="C318" t="s">
-        <v>868</v>
+        <v>875</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10655,16 +10709,19 @@
       <c r="G318">
         <v>0</v>
       </c>
-    </row>
-    <row r="319" spans="1:7">
+      <c r="H318" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8">
       <c r="A319" t="s">
-        <v>869</v>
+        <v>877</v>
       </c>
       <c r="B319" t="s">
-        <v>870</v>
+        <v>878</v>
       </c>
       <c r="C319" t="s">
-        <v>871</v>
+        <v>879</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10678,16 +10735,19 @@
       <c r="G319">
         <v>0</v>
       </c>
-    </row>
-    <row r="320" spans="1:7">
+      <c r="H319" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8">
       <c r="A320" t="s">
-        <v>872</v>
+        <v>881</v>
       </c>
       <c r="B320" t="s">
-        <v>873</v>
+        <v>882</v>
       </c>
       <c r="C320" t="s">
-        <v>873</v>
+        <v>882</v>
       </c>
       <c r="D320">
         <v>1</v>
@@ -10702,15 +10762,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:8">
       <c r="A321" t="s">
-        <v>874</v>
+        <v>883</v>
       </c>
       <c r="B321" t="s">
-        <v>875</v>
+        <v>884</v>
       </c>
       <c r="C321" t="s">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -10722,18 +10782,18 @@
         <v>0.99999833756146872</v>
       </c>
       <c r="G321">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8">
       <c r="A322" t="s">
-        <v>877</v>
+        <v>886</v>
       </c>
       <c r="B322" t="s">
-        <v>878</v>
+        <v>887</v>
       </c>
       <c r="C322" t="s">
-        <v>879</v>
+        <v>888</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -10745,18 +10805,18 @@
         <v>0.9924834523765006</v>
       </c>
       <c r="G322">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="323" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8">
       <c r="A323" t="s">
-        <v>880</v>
+        <v>889</v>
       </c>
       <c r="B323" t="s">
-        <v>881</v>
+        <v>890</v>
       </c>
       <c r="C323" t="s">
-        <v>882</v>
+        <v>891</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -10768,18 +10828,18 @@
         <v>0.99728739672709366</v>
       </c>
       <c r="G323">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="324" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8">
       <c r="A324" t="s">
-        <v>883</v>
+        <v>892</v>
       </c>
       <c r="B324" t="s">
-        <v>884</v>
+        <v>893</v>
       </c>
       <c r="C324" t="s">
-        <v>885</v>
+        <v>894</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10791,18 +10851,18 @@
         <v>0.99690437876548454</v>
       </c>
       <c r="G324">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8">
       <c r="A325" t="s">
-        <v>886</v>
+        <v>895</v>
       </c>
       <c r="B325" t="s">
-        <v>887</v>
+        <v>896</v>
       </c>
       <c r="C325" t="s">
-        <v>888</v>
+        <v>897</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10814,18 +10874,18 @@
         <v>0.9999968246710359</v>
       </c>
       <c r="G325">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="326" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8">
       <c r="A326" t="s">
-        <v>889</v>
+        <v>898</v>
       </c>
       <c r="B326" t="s">
-        <v>890</v>
+        <v>899</v>
       </c>
       <c r="C326" t="s">
-        <v>891</v>
+        <v>900</v>
       </c>
       <c r="D326">
         <v>0</v>
@@ -10839,16 +10899,19 @@
       <c r="G326">
         <v>0</v>
       </c>
-    </row>
-    <row r="327" spans="1:7">
+      <c r="H326" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8">
       <c r="A327" t="s">
-        <v>892</v>
+        <v>902</v>
       </c>
       <c r="B327" t="s">
-        <v>893</v>
+        <v>903</v>
       </c>
       <c r="C327" t="s">
-        <v>893</v>
+        <v>903</v>
       </c>
       <c r="D327">
         <v>1</v>

</xml_diff>